<commit_message>
Requirement & User stories updated by Kirubaharan
</commit_message>
<xml_diff>
--- a/Requirements/Requirements & User Flow.xlsx
+++ b/Requirements/Requirements & User Flow.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25203"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29B56C85-6DE7-4545-A02C-F387EF783D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{93560E72-F9C2-45D1-877E-89B409EF99D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="387">
   <si>
     <t>User story ID</t>
   </si>
@@ -469,6 +469,15 @@
   </si>
   <si>
     <t>MOM must be visible to Training coordinator and reviewer</t>
+  </si>
+  <si>
+    <t>As a trainee i should logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trainee can logout </t>
+  </si>
+  <si>
+    <t>Redirect to login page</t>
   </si>
   <si>
     <t>internal/external Trainer</t>
@@ -818,9 +827,6 @@
 Course should be created and added to the course list</t>
   </si>
   <si>
-    <t>Created course is added to the course list that can be viewed by trainee and trainer</t>
-  </si>
-  <si>
     <t>Training co ordinator should have the course name,course description,course duration.</t>
   </si>
   <si>
@@ -833,10 +839,16 @@
 Trainee should be able to view the course details</t>
   </si>
   <si>
-    <t>There should be atleast one trainee .There should be atleast one trainer.There should atleast one course.</t>
+    <t xml:space="preserve">
+There should be atleast one trainer.
+There should atleast one course.</t>
   </si>
   <si>
     <t>6) As a Training Co-ordinator i want to view the courses  so that i can assign trainer to course</t>
+  </si>
+  <si>
+    <t>There should be atleast one trainer.
+There should atleast one course.</t>
   </si>
   <si>
     <t>7) As a Training Co-ordinator  i want to monitor the trainee so that i can see the progress of the trainee</t>
@@ -847,6 +859,12 @@
 Training Co-ordinator can see the feed back of  the trainee about the course</t>
   </si>
   <si>
+    <t>Continous tracking will be done by the training co ordinator to know the performance of the trainee</t>
+  </si>
+  <si>
+    <t>Training Co-ordinator should be able to know the course progress of the trainee</t>
+  </si>
+  <si>
     <t>8) As a Training Co-ordinator i want to see the status of the course so that i can know the progress of the course .</t>
   </si>
   <si>
@@ -854,7 +872,7 @@
 Trainer should update the topics completed status or in progress status.</t>
   </si>
   <si>
-    <t>There should be atleast one course .</t>
+    <t>There should be atleast one course . Trainer should be assigned to the course .Trainer should update the topics completed status.</t>
   </si>
   <si>
     <t>9)As a Training Co-ordinator i want to Schedule review to the Reviewer so that the Reviewer can analyse the performance of the trainee.</t>
@@ -865,6 +883,13 @@
 Training co-ordinator should know the reviewe date 
 Training co-ordinator should send the notification about the review to reviewer and trainee
 Reviewer and trainee should receive the notification.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A report with the trainee's feedback will be created </t>
+  </si>
+  <si>
+    <t>There should be atleast one reviewer.
+There should atleast one trainee.</t>
   </si>
   <si>
     <t>Training co-ordinator</t>
@@ -1567,7 +1592,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1613,6 +1638,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1622,34 +1665,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1659,12 +1681,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1676,13 +1692,25 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -29060,10 +29088,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U271"/>
+  <dimension ref="A1:U274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
-      <selection activeCell="D272" sqref="D272"/>
+    <sheetView tabSelected="1" topLeftCell="A255" workbookViewId="0">
+      <selection activeCell="D274" sqref="D274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -29997,8 +30025,24 @@
       <c r="C271" t="s">
         <v>144</v>
       </c>
-      <c r="D271" s="2" t="s">
+      <c r="D271" s="5" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3">
+      <c r="A273" t="s">
+        <v>145</v>
+      </c>
+      <c r="B273" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3">
+      <c r="B274" t="s">
+        <v>146</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -30014,7 +30058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A29A159-1DDF-4514-8C0F-74BD61563D65}">
   <dimension ref="A3:U207"/>
   <sheetViews>
-    <sheetView topLeftCell="A197" workbookViewId="0">
+    <sheetView topLeftCell="A196" workbookViewId="0">
       <selection activeCell="C203" sqref="C203"/>
     </sheetView>
   </sheetViews>
@@ -30047,13 +30091,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C5" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D5" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -30061,13 +30105,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C6" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D6" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -30075,13 +30119,13 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C7" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D7" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -30089,13 +30133,13 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C8" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D8" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -30103,13 +30147,13 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C9" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D9" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -30117,13 +30161,13 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C10" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="D10" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -30131,13 +30175,13 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C11" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D11" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -30145,13 +30189,13 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C12" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D12" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -30159,13 +30203,13 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C13" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D13" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -30173,7 +30217,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
@@ -30189,7 +30233,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="B19" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="27" customHeight="1">
@@ -30239,7 +30283,7 @@
     </row>
     <row r="62" spans="10:10">
       <c r="J62" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="74" spans="2:5" ht="18.75">
@@ -30261,61 +30305,61 @@
         <v>1</v>
       </c>
       <c r="C75" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D75" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E75" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="76" spans="2:5">
       <c r="D76" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E76" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="77" spans="2:5">
       <c r="D77" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E77" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="78" spans="2:5">
       <c r="D78" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E78" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="80" spans="2:5">
       <c r="D80" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="E80" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="81" spans="4:5">
       <c r="D81" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E81" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="82" spans="4:5">
       <c r="D82" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E82" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="119" spans="1:15" ht="33" customHeight="1">
@@ -30361,27 +30405,27 @@
     </row>
     <row r="125" spans="1:15">
       <c r="A125" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="126" spans="1:15">
       <c r="A126" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="127" spans="1:15">
       <c r="A127" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="128" spans="1:15">
       <c r="A128" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="26.25">
@@ -30391,27 +30435,27 @@
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="C144" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -30426,15 +30470,15 @@
     </row>
     <row r="148" spans="1:4">
       <c r="B148" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D148" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="21">
       <c r="A153" s="4" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="21">
@@ -30469,10 +30513,10 @@
     </row>
     <row r="188" spans="1:21">
       <c r="A188" s="12" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B188" s="12" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C188" s="12" t="s">
         <v>35</v>
@@ -30483,13 +30527,13 @@
     </row>
     <row r="190" spans="1:21">
       <c r="A190" s="29" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B190" s="29" t="s">
         <v>51</v>
       </c>
       <c r="C190" s="29" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D190" s="29" t="s">
         <v>89</v>
@@ -30501,7 +30545,7 @@
         <v>52</v>
       </c>
       <c r="C191" s="29" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D191" s="29" t="s">
         <v>89</v>
@@ -30510,7 +30554,7 @@
     <row r="192" spans="1:21">
       <c r="A192" s="29"/>
       <c r="B192" s="29" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C192" s="29" t="s">
         <v>92</v>
@@ -30521,16 +30565,16 @@
     </row>
     <row r="194" spans="1:4">
       <c r="A194" s="29" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B194" s="29" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C194" s="29" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D194" s="29" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -30538,10 +30582,10 @@
         <v>110</v>
       </c>
       <c r="C195" s="29" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D195" s="29" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -30552,38 +30596,38 @@
     </row>
     <row r="199" spans="1:4">
       <c r="A199" s="30" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B199" s="29" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C199" s="29" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D199" s="29" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="200" spans="1:4">
       <c r="B200" s="29" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C200" s="29" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D200" s="29" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="203" spans="1:4">
       <c r="A203" s="29" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B203" s="29" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C203" s="29" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D203" s="29" t="s">
         <v>130</v>
@@ -30591,27 +30635,27 @@
     </row>
     <row r="204" spans="1:4">
       <c r="B204" s="29" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C204" s="29" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D204" s="29" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="207" spans="1:4">
       <c r="A207" s="29" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B207" s="29" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C207" s="29" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="D207" s="29" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -30662,13 +30706,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C3" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="D3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -30676,13 +30720,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C4" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D4" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -30690,13 +30734,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C5" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D5" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -30704,13 +30748,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C6" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="D6" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -30718,13 +30762,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C7" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D7" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -30732,13 +30776,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C8" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D8" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -30746,13 +30790,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C9" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D9" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -30760,13 +30804,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C10" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="D10" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -30774,13 +30818,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C11" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D11" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -30788,13 +30832,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C12" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D12" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -30802,13 +30846,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C13" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D13" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="18.75">
@@ -30820,7 +30864,7 @@
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="9" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -30848,13 +30892,13 @@
     </row>
     <row r="120" spans="5:5">
       <c r="E120" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="160" spans="1:18" ht="36.75" customHeight="1">
       <c r="A160" s="16"/>
       <c r="B160" s="16" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C160" s="19" t="s">
         <v>33</v>
@@ -30901,7 +30945,7 @@
     <row r="449" spans="2:19" ht="33.75">
       <c r="B449" s="16"/>
       <c r="C449" s="16" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="D449" s="19" t="s">
         <v>85</v>
@@ -30944,10 +30988,10 @@
     </row>
     <row r="457" spans="2:19">
       <c r="C457" s="28" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D457" s="28" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E457" s="28" t="s">
         <v>35</v>
@@ -30957,288 +31001,296 @@
       </c>
     </row>
     <row r="458" spans="2:19" ht="25.5" customHeight="1">
-      <c r="C458" s="53" t="s">
-        <v>246</v>
-      </c>
-      <c r="D458" s="62" t="s">
-        <v>247</v>
-      </c>
-      <c r="E458" s="44"/>
-      <c r="F458" s="69" t="s">
-        <v>248</v>
+      <c r="C458" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="D458" s="59" t="s">
+        <v>250</v>
+      </c>
+      <c r="E458" s="50"/>
+      <c r="F458" s="70" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="459" spans="2:19" ht="18.75" customHeight="1">
-      <c r="C459" s="48"/>
-      <c r="D459" s="63"/>
-      <c r="E459" s="45"/>
-      <c r="F459" s="70"/>
+      <c r="C459" s="45"/>
+      <c r="D459" s="60"/>
+      <c r="E459" s="51"/>
+      <c r="F459" s="71"/>
     </row>
     <row r="460" spans="2:19">
-      <c r="C460" s="48"/>
-      <c r="D460" s="63"/>
-      <c r="E460" s="45"/>
-      <c r="F460" s="70"/>
+      <c r="C460" s="45"/>
+      <c r="D460" s="60"/>
+      <c r="E460" s="51"/>
+      <c r="F460" s="71"/>
     </row>
     <row r="461" spans="2:19">
       <c r="C461" s="49"/>
-      <c r="D461" s="64"/>
-      <c r="E461" s="46"/>
-      <c r="F461" s="70"/>
+      <c r="D461" s="61"/>
+      <c r="E461" s="52"/>
+      <c r="F461" s="71"/>
     </row>
     <row r="462" spans="2:19" ht="15" customHeight="1">
-      <c r="C462" s="53" t="s">
-        <v>249</v>
-      </c>
-      <c r="D462" s="47" t="s">
-        <v>250</v>
-      </c>
-      <c r="E462" s="65" t="s">
-        <v>251</v>
-      </c>
-      <c r="F462" s="53" t="s">
+      <c r="C462" s="44" t="s">
         <v>252</v>
       </c>
+      <c r="D462" s="65" t="s">
+        <v>253</v>
+      </c>
+      <c r="E462" s="46" t="s">
+        <v>254</v>
+      </c>
+      <c r="F462" s="44" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="463" spans="2:19">
-      <c r="C463" s="48"/>
-      <c r="D463" s="50"/>
-      <c r="E463" s="66"/>
-      <c r="F463" s="48"/>
+      <c r="C463" s="45"/>
+      <c r="D463" s="66"/>
+      <c r="E463" s="47"/>
+      <c r="F463" s="45"/>
     </row>
     <row r="464" spans="2:19">
-      <c r="C464" s="48"/>
-      <c r="D464" s="50"/>
-      <c r="E464" s="66"/>
-      <c r="F464" s="48"/>
+      <c r="C464" s="45"/>
+      <c r="D464" s="66"/>
+      <c r="E464" s="47"/>
+      <c r="F464" s="45"/>
     </row>
     <row r="465" spans="3:6">
-      <c r="C465" s="48"/>
-      <c r="D465" s="50"/>
-      <c r="E465" s="66"/>
-      <c r="F465" s="48"/>
+      <c r="C465" s="45"/>
+      <c r="D465" s="66"/>
+      <c r="E465" s="47"/>
+      <c r="F465" s="45"/>
     </row>
     <row r="466" spans="3:6">
       <c r="C466" s="49"/>
-      <c r="D466" s="51"/>
-      <c r="E466" s="67"/>
+      <c r="D466" s="67"/>
+      <c r="E466" s="48"/>
       <c r="F466" s="49"/>
     </row>
     <row r="467" spans="3:6">
-      <c r="C467" s="53" t="s">
+      <c r="C467" s="44" t="s">
+        <v>256</v>
+      </c>
+      <c r="D467" s="68" t="s">
         <v>253</v>
       </c>
-      <c r="D467" s="52" t="s">
-        <v>250</v>
-      </c>
-      <c r="E467" s="54" t="s">
-        <v>254</v>
-      </c>
-      <c r="F467" s="48" t="s">
-        <v>255</v>
+      <c r="E467" s="62" t="s">
+        <v>257</v>
+      </c>
+      <c r="F467" s="45" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="468" spans="3:6">
-      <c r="C468" s="48"/>
-      <c r="D468" s="74"/>
-      <c r="E468" s="55"/>
-      <c r="F468" s="48"/>
+      <c r="C468" s="45"/>
+      <c r="D468" s="75"/>
+      <c r="E468" s="63"/>
+      <c r="F468" s="45"/>
     </row>
     <row r="469" spans="3:6">
       <c r="C469" s="49"/>
-      <c r="D469" s="74"/>
-      <c r="E469" s="56"/>
+      <c r="D469" s="75"/>
+      <c r="E469" s="64"/>
       <c r="F469" s="49"/>
     </row>
     <row r="470" spans="3:6">
-      <c r="C470" s="53" t="s">
-        <v>256</v>
-      </c>
-      <c r="D470" s="47" t="s">
-        <v>257</v>
-      </c>
-      <c r="E470" s="53" t="s">
-        <v>258</v>
-      </c>
-      <c r="F470" s="68" t="s">
+      <c r="C470" s="44" t="s">
         <v>259</v>
       </c>
+      <c r="D470" s="65" t="s">
+        <v>260</v>
+      </c>
+      <c r="E470" s="44"/>
+      <c r="F470" s="69" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="471" spans="3:6">
-      <c r="C471" s="48"/>
-      <c r="D471" s="48"/>
-      <c r="E471" s="48"/>
-      <c r="F471" s="72"/>
+      <c r="C471" s="45"/>
+      <c r="D471" s="45"/>
+      <c r="E471" s="45"/>
+      <c r="F471" s="73"/>
     </row>
     <row r="472" spans="3:6">
-      <c r="C472" s="48"/>
-      <c r="D472" s="48"/>
-      <c r="E472" s="48"/>
-      <c r="F472" s="72"/>
+      <c r="C472" s="45"/>
+      <c r="D472" s="45"/>
+      <c r="E472" s="45"/>
+      <c r="F472" s="73"/>
     </row>
     <row r="473" spans="3:6">
-      <c r="C473" s="48"/>
-      <c r="D473" s="48"/>
-      <c r="E473" s="48"/>
-      <c r="F473" s="72"/>
+      <c r="C473" s="45"/>
+      <c r="D473" s="45"/>
+      <c r="E473" s="45"/>
+      <c r="F473" s="73"/>
     </row>
     <row r="474" spans="3:6">
       <c r="C474" s="49"/>
       <c r="D474" s="49"/>
       <c r="E474" s="49"/>
-      <c r="F474" s="73"/>
+      <c r="F474" s="74"/>
     </row>
     <row r="475" spans="3:6">
-      <c r="C475" s="53" t="s">
-        <v>260</v>
-      </c>
-      <c r="D475" s="68" t="s">
-        <v>261</v>
-      </c>
-      <c r="E475" s="57"/>
-      <c r="F475" s="68" t="s">
+      <c r="C475" s="44" t="s">
         <v>262</v>
       </c>
+      <c r="D475" s="69" t="s">
+        <v>263</v>
+      </c>
+      <c r="E475" s="56"/>
+      <c r="F475" s="69" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="476" spans="3:6">
-      <c r="C476" s="48"/>
-      <c r="D476" s="60"/>
-      <c r="E476" s="58"/>
-      <c r="F476" s="72"/>
+      <c r="C476" s="45"/>
+      <c r="D476" s="54"/>
+      <c r="E476" s="57"/>
+      <c r="F476" s="73"/>
     </row>
     <row r="477" spans="3:6">
-      <c r="C477" s="48"/>
-      <c r="D477" s="60"/>
-      <c r="E477" s="58"/>
-      <c r="F477" s="72"/>
+      <c r="C477" s="45"/>
+      <c r="D477" s="54"/>
+      <c r="E477" s="57"/>
+      <c r="F477" s="73"/>
     </row>
     <row r="478" spans="3:6">
-      <c r="C478" s="48"/>
-      <c r="D478" s="60"/>
-      <c r="E478" s="58"/>
-      <c r="F478" s="72"/>
+      <c r="C478" s="45"/>
+      <c r="D478" s="54"/>
+      <c r="E478" s="57"/>
+      <c r="F478" s="73"/>
     </row>
     <row r="479" spans="3:6">
       <c r="C479" s="49"/>
-      <c r="D479" s="61"/>
-      <c r="E479" s="59"/>
-      <c r="F479" s="73"/>
+      <c r="D479" s="55"/>
+      <c r="E479" s="58"/>
+      <c r="F479" s="74"/>
     </row>
     <row r="480" spans="3:6">
-      <c r="C480" s="48" t="s">
+      <c r="C480" s="45" t="s">
+        <v>265</v>
+      </c>
+      <c r="D480" s="59" t="s">
         <v>263</v>
       </c>
-      <c r="D480" s="62" t="s">
-        <v>261</v>
-      </c>
-      <c r="E480" s="44"/>
-      <c r="F480" s="44"/>
+      <c r="E480" s="50"/>
+      <c r="F480" s="69" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="481" spans="2:6">
-      <c r="C481" s="48"/>
-      <c r="D481" s="63"/>
-      <c r="E481" s="45"/>
-      <c r="F481" s="45"/>
+      <c r="C481" s="45"/>
+      <c r="D481" s="60"/>
+      <c r="E481" s="51"/>
+      <c r="F481" s="54"/>
     </row>
     <row r="482" spans="2:6">
-      <c r="C482" s="48"/>
-      <c r="D482" s="63"/>
-      <c r="E482" s="45"/>
-      <c r="F482" s="45"/>
+      <c r="C482" s="45"/>
+      <c r="D482" s="60"/>
+      <c r="E482" s="51"/>
+      <c r="F482" s="54"/>
     </row>
     <row r="483" spans="2:6">
       <c r="C483" s="49"/>
-      <c r="D483" s="64"/>
-      <c r="E483" s="46"/>
-      <c r="F483" s="46"/>
+      <c r="D483" s="61"/>
+      <c r="E483" s="52"/>
+      <c r="F483" s="55"/>
     </row>
     <row r="484" spans="2:6">
-      <c r="C484" s="53" t="s">
-        <v>264</v>
-      </c>
-      <c r="D484" s="62" t="s">
-        <v>265</v>
-      </c>
-      <c r="E484" s="44"/>
-      <c r="F484" s="44"/>
+      <c r="C484" s="44" t="s">
+        <v>267</v>
+      </c>
+      <c r="D484" s="59" t="s">
+        <v>268</v>
+      </c>
+      <c r="E484" s="69" t="s">
+        <v>269</v>
+      </c>
+      <c r="F484" s="69" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="485" spans="2:6" ht="17.25" customHeight="1">
       <c r="B485" s="20"/>
-      <c r="C485" s="48"/>
-      <c r="D485" s="63"/>
-      <c r="E485" s="45"/>
-      <c r="F485" s="45"/>
+      <c r="C485" s="45"/>
+      <c r="D485" s="60"/>
+      <c r="E485" s="73"/>
+      <c r="F485" s="73"/>
     </row>
     <row r="486" spans="2:6">
-      <c r="C486" s="48"/>
-      <c r="D486" s="63"/>
-      <c r="E486" s="45"/>
-      <c r="F486" s="45"/>
+      <c r="C486" s="45"/>
+      <c r="D486" s="60"/>
+      <c r="E486" s="73"/>
+      <c r="F486" s="73"/>
     </row>
     <row r="487" spans="2:6">
       <c r="C487" s="49"/>
-      <c r="D487" s="64"/>
-      <c r="E487" s="46"/>
-      <c r="F487" s="46"/>
+      <c r="D487" s="61"/>
+      <c r="E487" s="74"/>
+      <c r="F487" s="74"/>
     </row>
     <row r="488" spans="2:6">
-      <c r="C488" s="53" t="s">
-        <v>266</v>
-      </c>
-      <c r="D488" s="69" t="s">
-        <v>267</v>
-      </c>
-      <c r="E488" s="44"/>
-      <c r="F488" s="44" t="s">
-        <v>268</v>
+      <c r="C488" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="D488" s="70" t="s">
+        <v>272</v>
+      </c>
+      <c r="E488" s="50"/>
+      <c r="F488" s="69" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="489" spans="2:6">
-      <c r="C489" s="48"/>
-      <c r="D489" s="70"/>
-      <c r="E489" s="45"/>
-      <c r="F489" s="45"/>
+      <c r="C489" s="45"/>
+      <c r="D489" s="71"/>
+      <c r="E489" s="51"/>
+      <c r="F489" s="73"/>
     </row>
     <row r="490" spans="2:6">
-      <c r="C490" s="48"/>
-      <c r="D490" s="70"/>
-      <c r="E490" s="45"/>
-      <c r="F490" s="45"/>
+      <c r="C490" s="45"/>
+      <c r="D490" s="71"/>
+      <c r="E490" s="51"/>
+      <c r="F490" s="73"/>
     </row>
     <row r="491" spans="2:6">
       <c r="C491" s="49"/>
-      <c r="D491" s="71"/>
-      <c r="E491" s="46"/>
-      <c r="F491" s="46"/>
+      <c r="D491" s="72"/>
+      <c r="E491" s="52"/>
+      <c r="F491" s="74"/>
     </row>
     <row r="492" spans="2:6">
-      <c r="C492" s="53" t="s">
-        <v>269</v>
-      </c>
-      <c r="D492" s="62" t="s">
-        <v>270</v>
-      </c>
-      <c r="E492" s="44"/>
-      <c r="F492" s="44"/>
+      <c r="C492" s="44" t="s">
+        <v>274</v>
+      </c>
+      <c r="D492" s="59" t="s">
+        <v>275</v>
+      </c>
+      <c r="E492" s="53" t="s">
+        <v>276</v>
+      </c>
+      <c r="F492" s="69" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="493" spans="2:6">
-      <c r="C493" s="48"/>
-      <c r="D493" s="63"/>
-      <c r="E493" s="45"/>
-      <c r="F493" s="45"/>
+      <c r="C493" s="45"/>
+      <c r="D493" s="60"/>
+      <c r="E493" s="54"/>
+      <c r="F493" s="54"/>
     </row>
     <row r="494" spans="2:6">
-      <c r="C494" s="48"/>
-      <c r="D494" s="63"/>
-      <c r="E494" s="45"/>
-      <c r="F494" s="45"/>
+      <c r="C494" s="45"/>
+      <c r="D494" s="60"/>
+      <c r="E494" s="54"/>
+      <c r="F494" s="54"/>
     </row>
     <row r="495" spans="2:6" ht="16.5" customHeight="1">
       <c r="B495" s="20"/>
       <c r="C495" s="49"/>
-      <c r="D495" s="64"/>
-      <c r="E495" s="46"/>
-      <c r="F495" s="46"/>
+      <c r="D495" s="61"/>
+      <c r="E495" s="55"/>
+      <c r="F495" s="55"/>
     </row>
     <row r="538" spans="1:2" ht="26.25">
       <c r="B538" s="20" t="s">
@@ -31247,30 +31299,30 @@
     </row>
     <row r="539" spans="1:2">
       <c r="A539" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="B539" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
     </row>
     <row r="540" spans="1:2">
       <c r="B540" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
     </row>
     <row r="541" spans="1:2">
       <c r="B541" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
     </row>
     <row r="542" spans="1:2">
       <c r="B542" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
     </row>
     <row r="546" spans="2:2">
       <c r="B546" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
     </row>
     <row r="548" spans="2:2" ht="26.25">
@@ -31288,22 +31340,22 @@
     </row>
     <row r="557" spans="2:2">
       <c r="B557" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
     </row>
     <row r="558" spans="2:2">
       <c r="B558" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
     </row>
     <row r="559" spans="2:2">
       <c r="B559" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
     </row>
     <row r="560" spans="2:2">
       <c r="B560" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
     </row>
     <row r="561" spans="2:2">
@@ -31313,7 +31365,7 @@
     </row>
     <row r="562" spans="2:2">
       <c r="B562" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="563" spans="2:2">
@@ -31323,22 +31375,22 @@
     </row>
     <row r="564" spans="2:2">
       <c r="B564" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
     </row>
     <row r="565" spans="2:2">
       <c r="B565" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
     </row>
     <row r="566" spans="2:2">
       <c r="B566" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
     </row>
     <row r="567" spans="2:2">
       <c r="B567" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
     </row>
     <row r="569" spans="2:2">
@@ -31348,7 +31400,7 @@
     </row>
     <row r="570" spans="2:2">
       <c r="B570" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="571" spans="2:2">
@@ -31358,17 +31410,17 @@
     </row>
     <row r="572" spans="2:2">
       <c r="B572" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
     </row>
     <row r="573" spans="2:2">
       <c r="B573" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
     </row>
     <row r="574" spans="2:2">
       <c r="B574" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
     </row>
     <row r="575" spans="2:2">
@@ -31378,12 +31430,12 @@
     </row>
     <row r="577" spans="2:2">
       <c r="B577" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
     </row>
     <row r="578" spans="2:2">
       <c r="B578" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
     </row>
     <row r="581" spans="2:2">
@@ -31393,22 +31445,19 @@
     </row>
     <row r="585" spans="2:2">
       <c r="B585" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="F458:F461"/>
-    <mergeCell ref="E462:E466"/>
-    <mergeCell ref="F462:F466"/>
-    <mergeCell ref="F467:F469"/>
-    <mergeCell ref="F488:F491"/>
-    <mergeCell ref="F475:F479"/>
-    <mergeCell ref="E480:E483"/>
-    <mergeCell ref="F480:F483"/>
-    <mergeCell ref="E484:E487"/>
-    <mergeCell ref="F484:F487"/>
-    <mergeCell ref="F470:F474"/>
+    <mergeCell ref="D470:D474"/>
+    <mergeCell ref="D462:D466"/>
+    <mergeCell ref="D467:D469"/>
+    <mergeCell ref="C484:C487"/>
+    <mergeCell ref="C488:C491"/>
+    <mergeCell ref="D488:D491"/>
+    <mergeCell ref="D492:D495"/>
+    <mergeCell ref="F492:F495"/>
     <mergeCell ref="C492:C495"/>
     <mergeCell ref="E458:E461"/>
     <mergeCell ref="E475:E479"/>
@@ -31425,15 +31474,18 @@
     <mergeCell ref="D458:D461"/>
     <mergeCell ref="C480:C483"/>
     <mergeCell ref="E470:E474"/>
+    <mergeCell ref="F458:F461"/>
+    <mergeCell ref="E462:E466"/>
+    <mergeCell ref="F462:F466"/>
+    <mergeCell ref="F467:F469"/>
+    <mergeCell ref="F488:F491"/>
+    <mergeCell ref="F475:F479"/>
+    <mergeCell ref="E480:E483"/>
+    <mergeCell ref="F480:F483"/>
+    <mergeCell ref="E484:E487"/>
+    <mergeCell ref="F484:F487"/>
+    <mergeCell ref="F470:F474"/>
     <mergeCell ref="E467:E469"/>
-    <mergeCell ref="C484:C487"/>
-    <mergeCell ref="C488:C491"/>
-    <mergeCell ref="D488:D491"/>
-    <mergeCell ref="D492:D495"/>
-    <mergeCell ref="F492:F495"/>
-    <mergeCell ref="D470:D474"/>
-    <mergeCell ref="D462:D466"/>
-    <mergeCell ref="D467:D469"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -31461,16 +31513,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="3" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -31478,13 +31530,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="C2" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="D2" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -31492,13 +31544,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="C3" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="D3" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -31506,13 +31558,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="C4" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="D4" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -31520,13 +31572,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="C5" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D5" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -31534,18 +31586,18 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="C6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D6" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="21">
       <c r="B18" s="4" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -31580,99 +31632,99 @@
     </row>
     <row r="32" spans="1:12">
       <c r="B32" s="5" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="C32" t="s">
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="E32" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="B33" s="5" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="C33" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="D33" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="E33" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="G33" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="14" customFormat="1">
       <c r="C34" s="14" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
     </row>
     <row r="35" spans="1:7" s="15" customFormat="1">
       <c r="A35" s="15" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="C36" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="D36" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="E36" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="D37" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="E37" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="E42" s="12" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="12" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -31680,7 +31732,7 @@
         <v>1</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -31688,7 +31740,7 @@
         <v>2</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -31696,7 +31748,7 @@
         <v>3</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
     </row>
     <row r="68" spans="1:14" ht="28.5" customHeight="1">
@@ -31735,16 +31787,16 @@
     </row>
     <row r="77" spans="1:14">
       <c r="B77" s="5" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="C77" t="s">
         <v>1</v>
       </c>
       <c r="D77" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="E77" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
     </row>
     <row r="78" spans="1:14">
@@ -31753,13 +31805,13 @@
         <v>1</v>
       </c>
       <c r="C78" s="24" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="D78" s="24" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="E78" s="24" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
     </row>
     <row r="79" spans="1:14">
@@ -31768,13 +31820,13 @@
         <v>2</v>
       </c>
       <c r="C79" s="24" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="D79" s="24" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="E79" s="24" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
     </row>
     <row r="80" spans="1:14">
@@ -31783,13 +31835,13 @@
         <v>3</v>
       </c>
       <c r="C80" s="24" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="D80" s="24" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="E80" s="24" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
     </row>
     <row r="81" spans="2:5">
@@ -31797,13 +31849,13 @@
         <v>4</v>
       </c>
       <c r="C81" s="24" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="D81" s="24" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
       <c r="E81" s="24" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
     </row>
     <row r="87" spans="2:5">
@@ -31847,10 +31899,10 @@
     </row>
     <row r="176" spans="1:15">
       <c r="B176" s="36" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C176" s="37" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D176" s="38" t="s">
         <v>35</v>
@@ -31861,35 +31913,35 @@
     </row>
     <row r="177" spans="2:5">
       <c r="B177" s="35" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="C177" s="28" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="D177" s="34" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="E177" s="33" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
     </row>
     <row r="178" spans="2:5">
       <c r="B178" s="35"/>
       <c r="C178" s="28" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="D178" s="34" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="E178" s="33"/>
     </row>
     <row r="179" spans="2:5">
       <c r="B179" s="40"/>
       <c r="C179" s="28" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="D179" s="42" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="E179" s="43"/>
     </row>
@@ -31901,25 +31953,25 @@
     </row>
     <row r="181" spans="2:5">
       <c r="B181" s="35" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="C181" s="28" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="D181" s="34" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="E181" s="33" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
     </row>
     <row r="182" spans="2:5">
       <c r="B182" s="35"/>
       <c r="C182" s="32" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="D182" s="34" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="E182" s="33"/>
     </row>
@@ -31931,23 +31983,23 @@
     </row>
     <row r="184" spans="2:5">
       <c r="B184" s="35" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
       <c r="C184" s="28" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="D184" s="34" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
       <c r="E184" s="33"/>
     </row>
     <row r="185" spans="2:5">
       <c r="B185" s="35"/>
       <c r="C185" s="28" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="D185" s="34" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="E185" s="33"/>
     </row>
@@ -31959,12 +32011,12 @@
     </row>
     <row r="187" spans="2:5">
       <c r="B187" s="40" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="C187" s="41"/>
       <c r="D187" s="42"/>
       <c r="E187" s="43" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -31985,7 +32037,7 @@
   <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -31998,7 +32050,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75">
@@ -32020,13 +32072,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="C4" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="D4" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -32034,13 +32086,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="C5" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="D5" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -32048,13 +32100,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="C6" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="D6" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -32062,13 +32114,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="C7" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="D7" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -32076,13 +32128,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="C8" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="D8" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -32090,13 +32142,13 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="C9" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="D9" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -32104,13 +32156,13 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="C10" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="D10" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -32118,13 +32170,13 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="C11" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="D11" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -32132,13 +32184,13 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="C12" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="D12" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -32146,13 +32198,13 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="C13" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D13" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -32160,13 +32212,13 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="C14" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="D14" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -32174,13 +32226,13 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="C15" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="D15" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18.75">
@@ -32190,7 +32242,7 @@
     </row>
     <row r="22" spans="1:5" ht="18.75">
       <c r="B22" s="1" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="18.75">
@@ -32198,7 +32250,7 @@
     </row>
     <row r="34" spans="1:17" ht="21">
       <c r="B34" s="4" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
     </row>
     <row r="41" spans="1:17" ht="29.25" customHeight="1">
@@ -32277,35 +32329,35 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="B2" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="39" customHeight="1">
       <c r="A9" s="17" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -32332,10 +32384,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Requirements updated by Sruthi
</commit_message>
<xml_diff>
--- a/Requirements/Requirements & User Flow.xlsx
+++ b/Requirements/Requirements & User Flow.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25131"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93560E72-F9C2-45D1-877E-89B409EF99D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D122574A-7B97-4418-BE63-D4F72D5C701B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="7" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trainee" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="389">
   <si>
     <t>User story ID</t>
   </si>
@@ -654,7 +654,7 @@
     <t>It can show time duration, Progress, List of trainees</t>
   </si>
   <si>
-    <t>Deatailed description about the course</t>
+    <t>Detailed description about the course</t>
   </si>
   <si>
     <t>As a trainer i want to view the List of topics</t>
@@ -703,6 +703,12 @@
   </si>
   <si>
     <t>Text box can hold upto 500 words</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trainer can logout </t>
+  </si>
+  <si>
+    <t>Trainer must be login</t>
   </si>
   <si>
     <t>Training Co-ordinator</t>
@@ -803,7 +809,7 @@
 Trainee should be able to login with the given credentials.</t>
   </si>
   <si>
-    <t>After registration , login credentials will be sent to the trainee Through mail.</t>
+    <t>After registration by training co ordinator, login credentials will be sent to the trainee Through mail.</t>
   </si>
   <si>
     <t>Training co ordinator should have  the trainee details.</t>
@@ -812,7 +818,7 @@
     <t>3) As a Training Co-ordinator i want to Register for trainer so that i can send the login credential through mail to the trainer.</t>
   </si>
   <si>
-    <t>After registration , login credentials will be sent to the trainer Through mail.</t>
+    <t>After registration  by training co ordinator, login credentials will be sent to the trainer Through mail.</t>
   </si>
   <si>
     <t>Training co ordinator should have  the trainer details.</t>
@@ -1358,24 +1364,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="20"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1622,9 +1628,7 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -1638,22 +1642,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1663,15 +1697,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1683,46 +1708,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1730,6 +1725,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -19828,7 +19834,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="TextBox 2">
+        <xdr:cNvPr id="17" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0FB878C-E557-432A-8308-2DC5F1184F5E}"/>
@@ -29090,8 +29096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A255" workbookViewId="0">
-      <selection activeCell="D274" sqref="D274"/>
+    <sheetView topLeftCell="A259" workbookViewId="0">
+      <selection activeCell="A273" sqref="A273:E274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30041,7 +30047,7 @@
       <c r="B274" t="s">
         <v>146</v>
       </c>
-      <c r="C274" s="2" t="s">
+      <c r="C274" s="5" t="s">
         <v>147</v>
       </c>
     </row>
@@ -30056,10 +30062,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A29A159-1DDF-4514-8C0F-74BD61563D65}">
-  <dimension ref="A3:U207"/>
+  <dimension ref="A3:U208"/>
   <sheetViews>
-    <sheetView topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="C203" sqref="C203"/>
+    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="A197" sqref="A197:XFD197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30525,137 +30531,221 @@
         <v>41</v>
       </c>
     </row>
-    <row r="190" spans="1:21">
-      <c r="A190" s="29" t="s">
+    <row r="189" spans="1:21" ht="15.75">
+      <c r="A189" s="73"/>
+      <c r="B189" s="73"/>
+      <c r="C189" s="73"/>
+      <c r="D189" s="73"/>
+      <c r="E189" s="73"/>
+    </row>
+    <row r="190" spans="1:21" ht="15.75">
+      <c r="A190" s="73" t="s">
         <v>197</v>
       </c>
-      <c r="B190" s="29" t="s">
+      <c r="B190" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="C190" s="29" t="s">
+      <c r="C190" s="73" t="s">
         <v>198</v>
       </c>
-      <c r="D190" s="29" t="s">
+      <c r="D190" s="73" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="191" spans="1:21">
-      <c r="A191" s="29"/>
-      <c r="B191" s="29" t="s">
+      <c r="E190" s="73"/>
+    </row>
+    <row r="191" spans="1:21" ht="15.75">
+      <c r="A191" s="73"/>
+      <c r="B191" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="C191" s="29" t="s">
+      <c r="C191" s="73" t="s">
         <v>199</v>
       </c>
-      <c r="D191" s="29" t="s">
+      <c r="D191" s="73" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="192" spans="1:21">
-      <c r="A192" s="29"/>
-      <c r="B192" s="29" t="s">
+      <c r="E191" s="73"/>
+    </row>
+    <row r="192" spans="1:21" ht="15.75">
+      <c r="A192" s="73"/>
+      <c r="B192" s="73" t="s">
         <v>200</v>
       </c>
-      <c r="C192" s="29" t="s">
+      <c r="C192" s="73" t="s">
         <v>92</v>
       </c>
-      <c r="D192" s="29" t="s">
+      <c r="D192" s="73" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="194" spans="1:4">
-      <c r="A194" s="29" t="s">
+      <c r="E192" s="73"/>
+    </row>
+    <row r="193" spans="1:5" ht="15.75">
+      <c r="A193" s="73"/>
+      <c r="B193" s="73"/>
+      <c r="C193" s="73"/>
+      <c r="D193" s="73"/>
+      <c r="E193" s="73"/>
+    </row>
+    <row r="194" spans="1:5" ht="15.75">
+      <c r="A194" s="73" t="s">
         <v>201</v>
       </c>
-      <c r="B194" s="29" t="s">
+      <c r="B194" s="73" t="s">
         <v>202</v>
       </c>
-      <c r="C194" s="29" t="s">
+      <c r="C194" s="73" t="s">
         <v>203</v>
       </c>
-      <c r="D194" s="29" t="s">
+      <c r="D194" s="73" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="195" spans="1:4">
-      <c r="B195" s="29" t="s">
+      <c r="E194" s="73"/>
+    </row>
+    <row r="195" spans="1:5" ht="15.75">
+      <c r="A195" s="73"/>
+      <c r="B195" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="C195" s="29" t="s">
+      <c r="C195" s="73" t="s">
         <v>205</v>
       </c>
-      <c r="D195" s="29" t="s">
+      <c r="D195" s="73" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="196" spans="1:4">
-      <c r="B196" s="29"/>
-    </row>
-    <row r="197" spans="1:4">
-      <c r="B197" s="29"/>
-    </row>
-    <row r="199" spans="1:4">
-      <c r="A199" s="30" t="s">
+      <c r="E195" s="73"/>
+    </row>
+    <row r="196" spans="1:5" ht="15.75">
+      <c r="A196" s="73"/>
+      <c r="B196" s="73"/>
+      <c r="C196" s="73"/>
+      <c r="D196" s="73"/>
+      <c r="E196" s="73"/>
+    </row>
+    <row r="197" spans="1:5" ht="15.75">
+      <c r="A197" s="73"/>
+      <c r="B197" s="73"/>
+      <c r="C197" s="73"/>
+      <c r="D197" s="73"/>
+      <c r="E197" s="73"/>
+    </row>
+    <row r="198" spans="1:5" ht="15.75">
+      <c r="A198" s="74" t="s">
         <v>207</v>
       </c>
-      <c r="B199" s="29" t="s">
+      <c r="B198" s="73" t="s">
         <v>208</v>
       </c>
-      <c r="C199" s="29" t="s">
+      <c r="C198" s="73" t="s">
         <v>203</v>
       </c>
-      <c r="D199" s="29" t="s">
+      <c r="D198" s="73" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="200" spans="1:4">
-      <c r="B200" s="29" t="s">
+      <c r="E198" s="73"/>
+    </row>
+    <row r="199" spans="1:5" ht="15.75">
+      <c r="A199" s="73"/>
+      <c r="B199" s="73" t="s">
         <v>210</v>
       </c>
-      <c r="C200" s="29" t="s">
+      <c r="C199" s="73" t="s">
         <v>211</v>
       </c>
-      <c r="D200" s="29" t="s">
+      <c r="D199" s="73" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="203" spans="1:4">
-      <c r="A203" s="29" t="s">
+      <c r="E199" s="73"/>
+    </row>
+    <row r="200" spans="1:5" ht="15.75">
+      <c r="A200" s="73"/>
+      <c r="B200" s="73"/>
+      <c r="C200" s="73"/>
+      <c r="D200" s="73"/>
+      <c r="E200" s="73"/>
+    </row>
+    <row r="201" spans="1:5" ht="15.75">
+      <c r="A201" s="73"/>
+      <c r="B201" s="73"/>
+      <c r="C201" s="73"/>
+      <c r="D201" s="73"/>
+      <c r="E201" s="73"/>
+    </row>
+    <row r="202" spans="1:5" ht="15.75">
+      <c r="A202" s="73" t="s">
         <v>213</v>
       </c>
-      <c r="B203" s="29" t="s">
+      <c r="B202" s="73" t="s">
         <v>214</v>
       </c>
-      <c r="C203" s="29" t="s">
+      <c r="C202" s="73" t="s">
         <v>215</v>
       </c>
-      <c r="D203" s="29" t="s">
+      <c r="D202" s="73" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="204" spans="1:4">
-      <c r="B204" s="29" t="s">
+      <c r="E202" s="73"/>
+    </row>
+    <row r="203" spans="1:5" ht="15.75">
+      <c r="A203" s="73"/>
+      <c r="B203" s="73" t="s">
         <v>216</v>
       </c>
-      <c r="C204" s="29" t="s">
+      <c r="C203" s="73" t="s">
         <v>217</v>
       </c>
-      <c r="D204" s="29" t="s">
+      <c r="D203" s="73" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="207" spans="1:4">
-      <c r="A207" s="29" t="s">
+      <c r="E203" s="73"/>
+    </row>
+    <row r="204" spans="1:5" ht="15.75">
+      <c r="A204" s="73"/>
+      <c r="B204" s="73"/>
+      <c r="C204" s="73"/>
+      <c r="D204" s="73"/>
+      <c r="E204" s="73"/>
+    </row>
+    <row r="205" spans="1:5" ht="15.75">
+      <c r="A205" s="73"/>
+      <c r="B205" s="73"/>
+      <c r="C205" s="73"/>
+      <c r="D205" s="73"/>
+      <c r="E205" s="73"/>
+    </row>
+    <row r="206" spans="1:5" ht="15.75">
+      <c r="A206" s="73" t="s">
         <v>219</v>
       </c>
-      <c r="B207" s="29" t="s">
+      <c r="B206" s="73" t="s">
         <v>220</v>
       </c>
-      <c r="C207" s="29" t="s">
+      <c r="C206" s="73" t="s">
         <v>221</v>
       </c>
-      <c r="D207" s="29" t="s">
+      <c r="D206" s="73" t="s">
         <v>222</v>
+      </c>
+      <c r="E206" s="73"/>
+    </row>
+    <row r="207" spans="1:5" ht="15.75">
+      <c r="A207" s="73"/>
+      <c r="B207" s="73"/>
+      <c r="C207" s="73"/>
+      <c r="D207" s="73"/>
+      <c r="E207" s="73"/>
+    </row>
+    <row r="208" spans="1:5">
+      <c r="A208" t="s">
+        <v>145</v>
+      </c>
+      <c r="B208" t="s">
+        <v>223</v>
+      </c>
+      <c r="C208" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D208" t="s">
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -30673,8 +30763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D891E2A-7FE3-4EFF-91F2-3D1BB267DA87}">
   <dimension ref="A2:S585"/>
   <sheetViews>
-    <sheetView topLeftCell="A449" workbookViewId="0">
-      <selection activeCell="D470" sqref="D470:D474"/>
+    <sheetView topLeftCell="D452" workbookViewId="0">
+      <selection activeCell="E462" sqref="E462:E466"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30706,13 +30796,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D3" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -30720,13 +30810,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D4" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -30734,13 +30824,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D5" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -30748,13 +30838,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C6" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D6" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -30762,13 +30852,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C7" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D7" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -30776,13 +30866,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C8" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D8" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -30790,13 +30880,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C9" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D9" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -30804,13 +30894,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C10" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D10" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -30818,13 +30908,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C11" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D11" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -30832,13 +30922,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C12" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D12" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -30846,13 +30936,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C13" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D13" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="18.75">
@@ -30864,7 +30954,7 @@
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="9" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -30892,13 +30982,13 @@
     </row>
     <row r="120" spans="5:5">
       <c r="E120" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="160" spans="1:18" ht="36.75" customHeight="1">
       <c r="A160" s="16"/>
       <c r="B160" s="16" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C160" s="19" t="s">
         <v>33</v>
@@ -30945,7 +31035,7 @@
     <row r="449" spans="2:19" ht="33.75">
       <c r="B449" s="16"/>
       <c r="C449" s="16" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D449" s="19" t="s">
         <v>85</v>
@@ -31001,296 +31091,296 @@
       </c>
     </row>
     <row r="458" spans="2:19" ht="25.5" customHeight="1">
-      <c r="C458" s="44" t="s">
-        <v>249</v>
-      </c>
-      <c r="D458" s="59" t="s">
-        <v>250</v>
-      </c>
-      <c r="E458" s="50"/>
-      <c r="F458" s="70" t="s">
+      <c r="C458" s="48" t="s">
         <v>251</v>
       </c>
+      <c r="D458" s="52" t="s">
+        <v>252</v>
+      </c>
+      <c r="E458" s="58"/>
+      <c r="F458" s="49" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="459" spans="2:19" ht="18.75" customHeight="1">
-      <c r="C459" s="45"/>
-      <c r="D459" s="60"/>
-      <c r="E459" s="51"/>
-      <c r="F459" s="71"/>
+      <c r="C459" s="43"/>
+      <c r="D459" s="53"/>
+      <c r="E459" s="59"/>
+      <c r="F459" s="50"/>
     </row>
     <row r="460" spans="2:19">
-      <c r="C460" s="45"/>
-      <c r="D460" s="60"/>
-      <c r="E460" s="51"/>
-      <c r="F460" s="71"/>
+      <c r="C460" s="43"/>
+      <c r="D460" s="53"/>
+      <c r="E460" s="59"/>
+      <c r="F460" s="50"/>
     </row>
     <row r="461" spans="2:19">
-      <c r="C461" s="49"/>
-      <c r="D461" s="61"/>
-      <c r="E461" s="52"/>
-      <c r="F461" s="71"/>
+      <c r="C461" s="44"/>
+      <c r="D461" s="54"/>
+      <c r="E461" s="60"/>
+      <c r="F461" s="50"/>
     </row>
     <row r="462" spans="2:19" ht="15" customHeight="1">
-      <c r="C462" s="44" t="s">
-        <v>252</v>
-      </c>
-      <c r="D462" s="65" t="s">
-        <v>253</v>
-      </c>
-      <c r="E462" s="46" t="s">
+      <c r="C462" s="48" t="s">
         <v>254</v>
       </c>
-      <c r="F462" s="44" t="s">
+      <c r="D462" s="42" t="s">
         <v>255</v>
       </c>
+      <c r="E462" s="65" t="s">
+        <v>256</v>
+      </c>
+      <c r="F462" s="48" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="463" spans="2:19">
-      <c r="C463" s="45"/>
-      <c r="D463" s="66"/>
-      <c r="E463" s="47"/>
-      <c r="F463" s="45"/>
+      <c r="C463" s="43"/>
+      <c r="D463" s="45"/>
+      <c r="E463" s="66"/>
+      <c r="F463" s="43"/>
     </row>
     <row r="464" spans="2:19">
-      <c r="C464" s="45"/>
-      <c r="D464" s="66"/>
-      <c r="E464" s="47"/>
-      <c r="F464" s="45"/>
+      <c r="C464" s="43"/>
+      <c r="D464" s="45"/>
+      <c r="E464" s="66"/>
+      <c r="F464" s="43"/>
     </row>
     <row r="465" spans="3:6">
-      <c r="C465" s="45"/>
-      <c r="D465" s="66"/>
-      <c r="E465" s="47"/>
-      <c r="F465" s="45"/>
+      <c r="C465" s="43"/>
+      <c r="D465" s="45"/>
+      <c r="E465" s="66"/>
+      <c r="F465" s="43"/>
     </row>
     <row r="466" spans="3:6">
-      <c r="C466" s="49"/>
-      <c r="D466" s="67"/>
-      <c r="E466" s="48"/>
-      <c r="F466" s="49"/>
+      <c r="C466" s="44"/>
+      <c r="D466" s="46"/>
+      <c r="E466" s="67"/>
+      <c r="F466" s="44"/>
     </row>
     <row r="467" spans="3:6">
-      <c r="C467" s="44" t="s">
-        <v>256</v>
-      </c>
-      <c r="D467" s="68" t="s">
-        <v>253</v>
-      </c>
-      <c r="E467" s="62" t="s">
-        <v>257</v>
-      </c>
-      <c r="F467" s="45" t="s">
+      <c r="C467" s="48" t="s">
         <v>258</v>
       </c>
+      <c r="D467" s="47" t="s">
+        <v>255</v>
+      </c>
+      <c r="E467" s="70" t="s">
+        <v>259</v>
+      </c>
+      <c r="F467" s="43" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="468" spans="3:6">
-      <c r="C468" s="45"/>
+      <c r="C468" s="43"/>
       <c r="D468" s="75"/>
-      <c r="E468" s="63"/>
-      <c r="F468" s="45"/>
+      <c r="E468" s="71"/>
+      <c r="F468" s="43"/>
     </row>
     <row r="469" spans="3:6">
-      <c r="C469" s="49"/>
+      <c r="C469" s="44"/>
       <c r="D469" s="75"/>
-      <c r="E469" s="64"/>
-      <c r="F469" s="49"/>
+      <c r="E469" s="72"/>
+      <c r="F469" s="44"/>
     </row>
     <row r="470" spans="3:6">
-      <c r="C470" s="44" t="s">
-        <v>259</v>
-      </c>
-      <c r="D470" s="65" t="s">
-        <v>260</v>
-      </c>
-      <c r="E470" s="44"/>
-      <c r="F470" s="69" t="s">
+      <c r="C470" s="48" t="s">
         <v>261</v>
       </c>
+      <c r="D470" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="E470" s="48"/>
+      <c r="F470" s="55" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="471" spans="3:6">
-      <c r="C471" s="45"/>
-      <c r="D471" s="45"/>
-      <c r="E471" s="45"/>
-      <c r="F471" s="73"/>
+      <c r="C471" s="43"/>
+      <c r="D471" s="43"/>
+      <c r="E471" s="43"/>
+      <c r="F471" s="68"/>
     </row>
     <row r="472" spans="3:6">
-      <c r="C472" s="45"/>
-      <c r="D472" s="45"/>
-      <c r="E472" s="45"/>
-      <c r="F472" s="73"/>
+      <c r="C472" s="43"/>
+      <c r="D472" s="43"/>
+      <c r="E472" s="43"/>
+      <c r="F472" s="68"/>
     </row>
     <row r="473" spans="3:6">
-      <c r="C473" s="45"/>
-      <c r="D473" s="45"/>
-      <c r="E473" s="45"/>
-      <c r="F473" s="73"/>
+      <c r="C473" s="43"/>
+      <c r="D473" s="43"/>
+      <c r="E473" s="43"/>
+      <c r="F473" s="68"/>
     </row>
     <row r="474" spans="3:6">
-      <c r="C474" s="49"/>
-      <c r="D474" s="49"/>
-      <c r="E474" s="49"/>
-      <c r="F474" s="74"/>
+      <c r="C474" s="44"/>
+      <c r="D474" s="44"/>
+      <c r="E474" s="44"/>
+      <c r="F474" s="69"/>
     </row>
     <row r="475" spans="3:6">
-      <c r="C475" s="44" t="s">
-        <v>262</v>
-      </c>
-      <c r="D475" s="69" t="s">
-        <v>263</v>
-      </c>
-      <c r="E475" s="56"/>
-      <c r="F475" s="69" t="s">
+      <c r="C475" s="48" t="s">
         <v>264</v>
       </c>
+      <c r="D475" s="55" t="s">
+        <v>265</v>
+      </c>
+      <c r="E475" s="61"/>
+      <c r="F475" s="55" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="476" spans="3:6">
-      <c r="C476" s="45"/>
-      <c r="D476" s="54"/>
-      <c r="E476" s="57"/>
-      <c r="F476" s="73"/>
+      <c r="C476" s="43"/>
+      <c r="D476" s="56"/>
+      <c r="E476" s="62"/>
+      <c r="F476" s="68"/>
     </row>
     <row r="477" spans="3:6">
-      <c r="C477" s="45"/>
-      <c r="D477" s="54"/>
-      <c r="E477" s="57"/>
-      <c r="F477" s="73"/>
+      <c r="C477" s="43"/>
+      <c r="D477" s="56"/>
+      <c r="E477" s="62"/>
+      <c r="F477" s="68"/>
     </row>
     <row r="478" spans="3:6">
-      <c r="C478" s="45"/>
-      <c r="D478" s="54"/>
-      <c r="E478" s="57"/>
-      <c r="F478" s="73"/>
+      <c r="C478" s="43"/>
+      <c r="D478" s="56"/>
+      <c r="E478" s="62"/>
+      <c r="F478" s="68"/>
     </row>
     <row r="479" spans="3:6">
-      <c r="C479" s="49"/>
-      <c r="D479" s="55"/>
-      <c r="E479" s="58"/>
-      <c r="F479" s="74"/>
+      <c r="C479" s="44"/>
+      <c r="D479" s="57"/>
+      <c r="E479" s="63"/>
+      <c r="F479" s="69"/>
     </row>
     <row r="480" spans="3:6">
-      <c r="C480" s="45" t="s">
+      <c r="C480" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="D480" s="52" t="s">
         <v>265</v>
       </c>
-      <c r="D480" s="59" t="s">
-        <v>263</v>
-      </c>
-      <c r="E480" s="50"/>
-      <c r="F480" s="69" t="s">
-        <v>266</v>
+      <c r="E480" s="58"/>
+      <c r="F480" s="55" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="481" spans="2:6">
-      <c r="C481" s="45"/>
-      <c r="D481" s="60"/>
-      <c r="E481" s="51"/>
-      <c r="F481" s="54"/>
+      <c r="C481" s="43"/>
+      <c r="D481" s="53"/>
+      <c r="E481" s="59"/>
+      <c r="F481" s="56"/>
     </row>
     <row r="482" spans="2:6">
-      <c r="C482" s="45"/>
-      <c r="D482" s="60"/>
-      <c r="E482" s="51"/>
-      <c r="F482" s="54"/>
+      <c r="C482" s="43"/>
+      <c r="D482" s="53"/>
+      <c r="E482" s="59"/>
+      <c r="F482" s="56"/>
     </row>
     <row r="483" spans="2:6">
-      <c r="C483" s="49"/>
-      <c r="D483" s="61"/>
-      <c r="E483" s="52"/>
-      <c r="F483" s="55"/>
+      <c r="C483" s="44"/>
+      <c r="D483" s="54"/>
+      <c r="E483" s="60"/>
+      <c r="F483" s="57"/>
     </row>
     <row r="484" spans="2:6">
-      <c r="C484" s="44" t="s">
-        <v>267</v>
-      </c>
-      <c r="D484" s="59" t="s">
-        <v>268</v>
-      </c>
-      <c r="E484" s="69" t="s">
+      <c r="C484" s="48" t="s">
         <v>269</v>
       </c>
-      <c r="F484" s="69" t="s">
+      <c r="D484" s="52" t="s">
         <v>270</v>
+      </c>
+      <c r="E484" s="55" t="s">
+        <v>271</v>
+      </c>
+      <c r="F484" s="55" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="485" spans="2:6" ht="17.25" customHeight="1">
       <c r="B485" s="20"/>
-      <c r="C485" s="45"/>
-      <c r="D485" s="60"/>
-      <c r="E485" s="73"/>
-      <c r="F485" s="73"/>
+      <c r="C485" s="43"/>
+      <c r="D485" s="53"/>
+      <c r="E485" s="68"/>
+      <c r="F485" s="68"/>
     </row>
     <row r="486" spans="2:6">
-      <c r="C486" s="45"/>
-      <c r="D486" s="60"/>
-      <c r="E486" s="73"/>
-      <c r="F486" s="73"/>
+      <c r="C486" s="43"/>
+      <c r="D486" s="53"/>
+      <c r="E486" s="68"/>
+      <c r="F486" s="68"/>
     </row>
     <row r="487" spans="2:6">
-      <c r="C487" s="49"/>
-      <c r="D487" s="61"/>
-      <c r="E487" s="74"/>
-      <c r="F487" s="74"/>
+      <c r="C487" s="44"/>
+      <c r="D487" s="54"/>
+      <c r="E487" s="69"/>
+      <c r="F487" s="69"/>
     </row>
     <row r="488" spans="2:6">
-      <c r="C488" s="44" t="s">
-        <v>271</v>
-      </c>
-      <c r="D488" s="70" t="s">
-        <v>272</v>
-      </c>
-      <c r="E488" s="50"/>
-      <c r="F488" s="69" t="s">
+      <c r="C488" s="48" t="s">
         <v>273</v>
       </c>
+      <c r="D488" s="49" t="s">
+        <v>274</v>
+      </c>
+      <c r="E488" s="58"/>
+      <c r="F488" s="55" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="489" spans="2:6">
-      <c r="C489" s="45"/>
-      <c r="D489" s="71"/>
-      <c r="E489" s="51"/>
-      <c r="F489" s="73"/>
+      <c r="C489" s="43"/>
+      <c r="D489" s="50"/>
+      <c r="E489" s="59"/>
+      <c r="F489" s="68"/>
     </row>
     <row r="490" spans="2:6">
-      <c r="C490" s="45"/>
-      <c r="D490" s="71"/>
-      <c r="E490" s="51"/>
-      <c r="F490" s="73"/>
+      <c r="C490" s="43"/>
+      <c r="D490" s="50"/>
+      <c r="E490" s="59"/>
+      <c r="F490" s="68"/>
     </row>
     <row r="491" spans="2:6">
-      <c r="C491" s="49"/>
-      <c r="D491" s="72"/>
-      <c r="E491" s="52"/>
-      <c r="F491" s="74"/>
+      <c r="C491" s="44"/>
+      <c r="D491" s="51"/>
+      <c r="E491" s="60"/>
+      <c r="F491" s="69"/>
     </row>
     <row r="492" spans="2:6">
-      <c r="C492" s="44" t="s">
-        <v>274</v>
-      </c>
-      <c r="D492" s="59" t="s">
-        <v>275</v>
-      </c>
-      <c r="E492" s="53" t="s">
+      <c r="C492" s="48" t="s">
         <v>276</v>
       </c>
-      <c r="F492" s="69" t="s">
+      <c r="D492" s="52" t="s">
         <v>277</v>
       </c>
+      <c r="E492" s="64" t="s">
+        <v>278</v>
+      </c>
+      <c r="F492" s="55" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="493" spans="2:6">
-      <c r="C493" s="45"/>
-      <c r="D493" s="60"/>
-      <c r="E493" s="54"/>
-      <c r="F493" s="54"/>
+      <c r="C493" s="43"/>
+      <c r="D493" s="53"/>
+      <c r="E493" s="56"/>
+      <c r="F493" s="56"/>
     </row>
     <row r="494" spans="2:6">
-      <c r="C494" s="45"/>
-      <c r="D494" s="60"/>
-      <c r="E494" s="54"/>
-      <c r="F494" s="54"/>
+      <c r="C494" s="43"/>
+      <c r="D494" s="53"/>
+      <c r="E494" s="56"/>
+      <c r="F494" s="56"/>
     </row>
     <row r="495" spans="2:6" ht="16.5" customHeight="1">
       <c r="B495" s="20"/>
-      <c r="C495" s="49"/>
-      <c r="D495" s="61"/>
-      <c r="E495" s="55"/>
-      <c r="F495" s="55"/>
+      <c r="C495" s="44"/>
+      <c r="D495" s="54"/>
+      <c r="E495" s="57"/>
+      <c r="F495" s="57"/>
     </row>
     <row r="538" spans="1:2" ht="26.25">
       <c r="B538" s="20" t="s">
@@ -31299,30 +31389,30 @@
     </row>
     <row r="539" spans="1:2">
       <c r="A539" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B539" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="540" spans="1:2">
       <c r="B540" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="541" spans="1:2">
       <c r="B541" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="542" spans="1:2">
       <c r="B542" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="546" spans="2:2">
       <c r="B546" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="548" spans="2:2" ht="26.25">
@@ -31340,22 +31430,22 @@
     </row>
     <row r="557" spans="2:2">
       <c r="B557" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="558" spans="2:2">
       <c r="B558" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="559" spans="2:2">
       <c r="B559" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="560" spans="2:2">
       <c r="B560" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="561" spans="2:2">
@@ -31365,7 +31455,7 @@
     </row>
     <row r="562" spans="2:2">
       <c r="B562" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="563" spans="2:2">
@@ -31375,22 +31465,22 @@
     </row>
     <row r="564" spans="2:2">
       <c r="B564" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="565" spans="2:2">
       <c r="B565" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="566" spans="2:2">
       <c r="B566" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="567" spans="2:2">
       <c r="B567" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="569" spans="2:2">
@@ -31400,7 +31490,7 @@
     </row>
     <row r="570" spans="2:2">
       <c r="B570" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="571" spans="2:2">
@@ -31410,17 +31500,17 @@
     </row>
     <row r="572" spans="2:2">
       <c r="B572" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="573" spans="2:2">
       <c r="B573" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="574" spans="2:2">
       <c r="B574" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="575" spans="2:2">
@@ -31430,12 +31520,12 @@
     </row>
     <row r="577" spans="2:2">
       <c r="B577" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="578" spans="2:2">
       <c r="B578" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="581" spans="2:2">
@@ -31445,17 +31535,24 @@
     </row>
     <row r="585" spans="2:2">
       <c r="B585" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="D470:D474"/>
-    <mergeCell ref="D462:D466"/>
-    <mergeCell ref="D467:D469"/>
-    <mergeCell ref="C484:C487"/>
-    <mergeCell ref="C488:C491"/>
-    <mergeCell ref="D488:D491"/>
+    <mergeCell ref="F488:F491"/>
+    <mergeCell ref="F475:F479"/>
+    <mergeCell ref="E480:E483"/>
+    <mergeCell ref="F480:F483"/>
+    <mergeCell ref="E484:E487"/>
+    <mergeCell ref="F484:F487"/>
+    <mergeCell ref="E470:E474"/>
+    <mergeCell ref="F458:F461"/>
+    <mergeCell ref="E462:E466"/>
+    <mergeCell ref="F462:F466"/>
+    <mergeCell ref="F467:F469"/>
+    <mergeCell ref="F470:F474"/>
+    <mergeCell ref="E467:E469"/>
     <mergeCell ref="D492:D495"/>
     <mergeCell ref="F492:F495"/>
     <mergeCell ref="C492:C495"/>
@@ -31472,20 +31569,13 @@
     <mergeCell ref="D480:D483"/>
     <mergeCell ref="D484:D487"/>
     <mergeCell ref="D458:D461"/>
+    <mergeCell ref="D470:D474"/>
+    <mergeCell ref="D462:D466"/>
+    <mergeCell ref="D467:D469"/>
+    <mergeCell ref="C484:C487"/>
+    <mergeCell ref="C488:C491"/>
+    <mergeCell ref="D488:D491"/>
     <mergeCell ref="C480:C483"/>
-    <mergeCell ref="E470:E474"/>
-    <mergeCell ref="F458:F461"/>
-    <mergeCell ref="E462:E466"/>
-    <mergeCell ref="F462:F466"/>
-    <mergeCell ref="F467:F469"/>
-    <mergeCell ref="F488:F491"/>
-    <mergeCell ref="F475:F479"/>
-    <mergeCell ref="E480:E483"/>
-    <mergeCell ref="F480:F483"/>
-    <mergeCell ref="E484:E487"/>
-    <mergeCell ref="F484:F487"/>
-    <mergeCell ref="F470:F474"/>
-    <mergeCell ref="E467:E469"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -31513,16 +31603,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="3" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -31530,13 +31620,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C2" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D2" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -31544,13 +31634,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C3" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="D3" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -31558,13 +31648,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C4" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D4" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -31572,13 +31662,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C5" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D5" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -31586,18 +31676,18 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C6" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D6" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="21">
       <c r="B18" s="4" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -31632,99 +31722,99 @@
     </row>
     <row r="32" spans="1:12">
       <c r="B32" s="5" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C32" t="s">
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="E32" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="B33" s="5" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="C33" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D33" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="E33" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="G33" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="14" customFormat="1">
       <c r="C34" s="14" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="35" spans="1:7" s="15" customFormat="1">
       <c r="A35" s="15" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="C36" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D36" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="E36" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="D37" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="E37" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="E42" s="12" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="12" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -31740,7 +31830,7 @@
         <v>2</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -31748,7 +31838,7 @@
         <v>3</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="68" spans="1:14" ht="28.5" customHeight="1">
@@ -31787,16 +31877,16 @@
     </row>
     <row r="77" spans="1:14">
       <c r="B77" s="5" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C77" t="s">
         <v>1</v>
       </c>
       <c r="D77" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="E77" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="78" spans="1:14">
@@ -31805,13 +31895,13 @@
         <v>1</v>
       </c>
       <c r="C78" s="24" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D78" s="24" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="E78" s="24" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="79" spans="1:14">
@@ -31820,13 +31910,13 @@
         <v>2</v>
       </c>
       <c r="C79" s="24" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D79" s="24" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="E79" s="24" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="80" spans="1:14">
@@ -31835,13 +31925,13 @@
         <v>3</v>
       </c>
       <c r="C80" s="24" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D80" s="24" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="E80" s="24" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="81" spans="2:5">
@@ -31849,13 +31939,13 @@
         <v>4</v>
       </c>
       <c r="C81" s="24" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D81" s="24" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="E81" s="24" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="87" spans="2:5">
@@ -31865,7 +31955,7 @@
       <c r="A171" s="16"/>
       <c r="B171" s="16"/>
       <c r="C171" s="16"/>
-      <c r="D171" s="31" t="s">
+      <c r="D171" s="29" t="s">
         <v>85</v>
       </c>
       <c r="E171" s="16"/>
@@ -31898,125 +31988,125 @@
       <c r="O172" s="16"/>
     </row>
     <row r="176" spans="1:15">
-      <c r="B176" s="36" t="s">
+      <c r="B176" s="34" t="s">
         <v>195</v>
       </c>
-      <c r="C176" s="37" t="s">
+      <c r="C176" s="35" t="s">
         <v>196</v>
       </c>
-      <c r="D176" s="38" t="s">
+      <c r="D176" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="E176" s="39" t="s">
+      <c r="E176" s="37" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="177" spans="2:5">
-      <c r="B177" s="35" t="s">
-        <v>331</v>
+      <c r="B177" s="33" t="s">
+        <v>333</v>
       </c>
       <c r="C177" s="28" t="s">
-        <v>332</v>
-      </c>
-      <c r="D177" s="34" t="s">
-        <v>333</v>
-      </c>
-      <c r="E177" s="33" t="s">
         <v>334</v>
       </c>
+      <c r="D177" s="32" t="s">
+        <v>335</v>
+      </c>
+      <c r="E177" s="31" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="178" spans="2:5">
-      <c r="B178" s="35"/>
+      <c r="B178" s="33"/>
       <c r="C178" s="28" t="s">
-        <v>335</v>
-      </c>
-      <c r="D178" s="34" t="s">
-        <v>336</v>
-      </c>
-      <c r="E178" s="33"/>
+        <v>337</v>
+      </c>
+      <c r="D178" s="32" t="s">
+        <v>338</v>
+      </c>
+      <c r="E178" s="31"/>
     </row>
     <row r="179" spans="2:5">
-      <c r="B179" s="40"/>
+      <c r="B179" s="38"/>
       <c r="C179" s="28" t="s">
-        <v>337</v>
-      </c>
-      <c r="D179" s="42" t="s">
-        <v>338</v>
-      </c>
-      <c r="E179" s="43"/>
+        <v>339</v>
+      </c>
+      <c r="D179" s="40" t="s">
+        <v>340</v>
+      </c>
+      <c r="E179" s="41"/>
     </row>
     <row r="180" spans="2:5">
-      <c r="B180" s="35"/>
+      <c r="B180" s="33"/>
       <c r="C180" s="28"/>
-      <c r="D180" s="34"/>
-      <c r="E180" s="33"/>
+      <c r="D180" s="32"/>
+      <c r="E180" s="31"/>
     </row>
     <row r="181" spans="2:5">
-      <c r="B181" s="35" t="s">
-        <v>339</v>
+      <c r="B181" s="33" t="s">
+        <v>341</v>
       </c>
       <c r="C181" s="28" t="s">
-        <v>340</v>
-      </c>
-      <c r="D181" s="34" t="s">
-        <v>341</v>
-      </c>
-      <c r="E181" s="33" t="s">
         <v>342</v>
       </c>
+      <c r="D181" s="32" t="s">
+        <v>343</v>
+      </c>
+      <c r="E181" s="31" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="182" spans="2:5">
-      <c r="B182" s="35"/>
-      <c r="C182" s="32" t="s">
-        <v>343</v>
-      </c>
-      <c r="D182" s="34" t="s">
-        <v>344</v>
-      </c>
-      <c r="E182" s="33"/>
+      <c r="B182" s="33"/>
+      <c r="C182" s="30" t="s">
+        <v>345</v>
+      </c>
+      <c r="D182" s="32" t="s">
+        <v>346</v>
+      </c>
+      <c r="E182" s="31"/>
     </row>
     <row r="183" spans="2:5">
-      <c r="B183" s="35"/>
+      <c r="B183" s="33"/>
       <c r="C183" s="28"/>
-      <c r="D183" s="34"/>
-      <c r="E183" s="33"/>
+      <c r="D183" s="32"/>
+      <c r="E183" s="31"/>
     </row>
     <row r="184" spans="2:5">
-      <c r="B184" s="35" t="s">
-        <v>345</v>
+      <c r="B184" s="33" t="s">
+        <v>347</v>
       </c>
       <c r="C184" s="28" t="s">
-        <v>346</v>
-      </c>
-      <c r="D184" s="34" t="s">
-        <v>347</v>
-      </c>
-      <c r="E184" s="33"/>
+        <v>348</v>
+      </c>
+      <c r="D184" s="32" t="s">
+        <v>349</v>
+      </c>
+      <c r="E184" s="31"/>
     </row>
     <row r="185" spans="2:5">
-      <c r="B185" s="35"/>
+      <c r="B185" s="33"/>
       <c r="C185" s="28" t="s">
-        <v>348</v>
-      </c>
-      <c r="D185" s="34" t="s">
-        <v>349</v>
-      </c>
-      <c r="E185" s="33"/>
+        <v>350</v>
+      </c>
+      <c r="D185" s="32" t="s">
+        <v>351</v>
+      </c>
+      <c r="E185" s="31"/>
     </row>
     <row r="186" spans="2:5">
-      <c r="B186" s="35"/>
+      <c r="B186" s="33"/>
       <c r="C186" s="28"/>
-      <c r="D186" s="34"/>
-      <c r="E186" s="33"/>
+      <c r="D186" s="32"/>
+      <c r="E186" s="31"/>
     </row>
     <row r="187" spans="2:5">
-      <c r="B187" s="40" t="s">
-        <v>350</v>
-      </c>
-      <c r="C187" s="41"/>
-      <c r="D187" s="42"/>
-      <c r="E187" s="43" t="s">
-        <v>351</v>
+      <c r="B187" s="38" t="s">
+        <v>352</v>
+      </c>
+      <c r="C187" s="39"/>
+      <c r="D187" s="40"/>
+      <c r="E187" s="41" t="s">
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -32037,7 +32127,7 @@
   <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32050,7 +32140,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75">
@@ -32072,13 +32162,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C4" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="D4" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -32086,13 +32176,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C5" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="D5" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -32100,13 +32190,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C6" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="D6" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -32114,13 +32204,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C7" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="D7" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -32128,13 +32218,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C8" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D8" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -32142,13 +32232,13 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C9" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="D9" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -32156,13 +32246,13 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C10" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="D10" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -32170,13 +32260,13 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C11" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D11" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -32184,13 +32274,13 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C12" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="D12" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -32198,7 +32288,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C13" t="s">
         <v>161</v>
@@ -32212,13 +32302,13 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C14" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="D14" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -32226,13 +32316,13 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C15" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="D15" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18.75">
@@ -32242,7 +32332,7 @@
     </row>
     <row r="22" spans="1:5" ht="18.75">
       <c r="B22" s="1" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="18.75">
@@ -32250,7 +32340,7 @@
     </row>
     <row r="34" spans="1:17" ht="21">
       <c r="B34" s="4" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="41" spans="1:17" ht="29.25" customHeight="1">
@@ -32329,35 +32419,35 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B2" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="39" customHeight="1">
       <c r="A9" s="17" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -32381,13 +32471,16 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="167.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data entity and Figma prototype
</commit_message>
<xml_diff>
--- a/Requirements/Requirements & User Flow.xlsx
+++ b/Requirements/Requirements & User Flow.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25203"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D122574A-7B97-4418-BE63-D4F72D5C701B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FCB26E7-8569-4E98-9D60-835ACE0AAF8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="7" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trainee" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,8 @@
     <sheet name="Flow Chart" sheetId="6" r:id="rId6"/>
     <sheet name="Queries" sheetId="7" r:id="rId7"/>
     <sheet name="Timesheets" sheetId="8" r:id="rId8"/>
+    <sheet name="Data Model" sheetId="10" r:id="rId9"/>
+    <sheet name="Figma" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="403">
   <si>
     <t>User story ID</t>
   </si>
@@ -309,334 +311,367 @@
     <t>If not it will not allow user to login</t>
   </si>
   <si>
-    <t>It navigate to the landing page</t>
+    <t xml:space="preserve">It navigate to the landing page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Landing page is common for all users </t>
+  </si>
+  <si>
+    <t>It should have assigned courses</t>
+  </si>
+  <si>
+    <t>It should view technology,trainer,duration of the assigned courses</t>
+  </si>
+  <si>
+    <t>All course may not be displayed in dashboard</t>
+  </si>
+  <si>
+    <t>It should have scheduled review</t>
+  </si>
+  <si>
+    <t>It should shows review details</t>
+  </si>
+  <si>
+    <t>Review should assigned by  Training cocrdinate</t>
+  </si>
+  <si>
+    <t>It should have search bar</t>
+  </si>
+  <si>
+    <t>It will help the trainee to find the course quickly</t>
+  </si>
+  <si>
+    <t>It should show attendance marking option</t>
+  </si>
+  <si>
+    <t>Trainee has to self mark the attendance status</t>
+  </si>
+  <si>
+    <t>Trainee must be enrolled in that course</t>
+  </si>
+  <si>
+    <t>It should contain topics related to the course</t>
+  </si>
+  <si>
+    <t>It can be video or document materials</t>
+  </si>
+  <si>
+    <t>Topics and  materials updated by trainer</t>
+  </si>
+  <si>
+    <t>It shows the trainer assigned to the course</t>
+  </si>
+  <si>
+    <t>It will show the trainer name</t>
+  </si>
+  <si>
+    <t>Trainer should be assigned by  Training coordinate</t>
+  </si>
+  <si>
+    <t>It contains course details</t>
+  </si>
+  <si>
+    <t>It shows (Duration, Course goals, Course description, Prerequisites)</t>
+  </si>
+  <si>
+    <t>Should be created during course  creation</t>
+  </si>
+  <si>
+    <t>Trainee can submit the attendance</t>
+  </si>
+  <si>
+    <t>It can be check box or dropdown</t>
+  </si>
+  <si>
+    <t>It will have limited time for marking the attendance</t>
+  </si>
+  <si>
+    <t>It could be 15-30 mins</t>
+  </si>
+  <si>
+    <t>Trainee can submit the feedback to trainer</t>
+  </si>
+  <si>
+    <t>It may be textbox can hold about 500 words</t>
+  </si>
+  <si>
+    <t>The input entered in the textbox should be view by Trainer and coordinator</t>
+  </si>
+  <si>
+    <t>Trainer must be assigned to the course</t>
+  </si>
+  <si>
+    <t>It contains filter option to get a details about feedback</t>
+  </si>
+  <si>
+    <t>It'll get date from the user</t>
+  </si>
+  <si>
+    <t>Date must be valid</t>
+  </si>
+  <si>
+    <t>It can be a grid or list view</t>
+  </si>
+  <si>
+    <t>Activity can be given on daily basis</t>
+  </si>
+  <si>
+    <t>It can be quiz or exploration</t>
+  </si>
+  <si>
+    <t>Activity should be submitted by individual</t>
+  </si>
+  <si>
+    <t>It contains questions as documents</t>
+  </si>
+  <si>
+    <t>trainee can download them</t>
+  </si>
+  <si>
+    <t>current assignment should be completed before the next one</t>
+  </si>
+  <si>
+    <t>Trainee cannot change the deadline</t>
+  </si>
+  <si>
+    <t>Assignments should be submitted before deadline</t>
+  </si>
+  <si>
+    <t>Trainee can upload both pdf and word document</t>
+  </si>
+  <si>
+    <t>Upload document size must be limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> It displays the marks scored </t>
+  </si>
+  <si>
+    <t>It may be overall mark scored or individual course</t>
+  </si>
+  <si>
+    <t>It contains details about the upcoming meeting</t>
+  </si>
+  <si>
+    <t>It should have the meeting link</t>
+  </si>
+  <si>
+    <t>Review must be scheduled by  Training cocrdinate</t>
+  </si>
+  <si>
+    <t>It may have meeting history</t>
+  </si>
+  <si>
+    <t>Review must be completed</t>
+  </si>
+  <si>
+    <t>The history of reviews will be shown</t>
+  </si>
+  <si>
+    <t>It contains text fields of Reviewer and date of review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It may be textbox or dropdown </t>
+  </si>
+  <si>
+    <t xml:space="preserve">It contains fields(actions to be done and meeting notes) </t>
+  </si>
+  <si>
+    <t>MOM must be visible to Training coordinator and reviewer</t>
+  </si>
+  <si>
+    <t>As a trainee i should logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trainee can logout </t>
+  </si>
+  <si>
+    <t>Redirect to login page</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> It navigate to the Dashboard</t>
+  </si>
+  <si>
+    <t>Landing page is common for all users ?? Home page</t>
+  </si>
+  <si>
+    <t>?? i have to receive the credentails mail first</t>
+  </si>
+  <si>
+    <t>It contains trainer assigned</t>
+  </si>
+  <si>
+    <t>It should update attendance</t>
+  </si>
+  <si>
+    <t>Only for specified time attendence will be available</t>
+  </si>
+  <si>
+    <t>Trainer can give his views about course and trainer</t>
+  </si>
+  <si>
+    <t>It contains filter option to sort feebacks of specific date</t>
+  </si>
+  <si>
+    <t>internal/external Trainer</t>
+  </si>
+  <si>
+    <t>teach course to the trainees</t>
+  </si>
+  <si>
+    <t>train them properly</t>
+  </si>
+  <si>
+    <t>make them understand the concepts</t>
+  </si>
+  <si>
+    <t>make them gain knowledge</t>
+  </si>
+  <si>
+    <t>plan the schedule</t>
+  </si>
+  <si>
+    <t>complete within the given time</t>
+  </si>
+  <si>
+    <t>guide them with the project</t>
+  </si>
+  <si>
+    <t>Push them for project review</t>
+  </si>
+  <si>
+    <t>conduct a clarification session</t>
+  </si>
+  <si>
+    <t>clarify their doubts</t>
+  </si>
+  <si>
+    <t>Monitor their works</t>
+  </si>
+  <si>
+    <t>know whats their progress</t>
+  </si>
+  <si>
+    <t>track attendence of trainee</t>
+  </si>
+  <si>
+    <t>report to higher ups</t>
+  </si>
+  <si>
+    <t>Provides feedback</t>
+  </si>
+  <si>
+    <t>make trainees improve themself</t>
+  </si>
+  <si>
+    <t>view status Update</t>
+  </si>
+  <si>
+    <t>track them on daily basis</t>
+  </si>
+  <si>
+    <t>Trainer - &gt; Register/Login - &gt;	Attendence - &gt; Plan the Course	- &gt; Assignments - &gt; Session Clarification - &gt; Feedback</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Trainer</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Enter into the assigned course</t>
+  </si>
+  <si>
+    <t>View the courses</t>
+  </si>
+  <si>
+    <t>see the course topics</t>
+  </si>
+  <si>
+    <t>View the topics</t>
+  </si>
+  <si>
+    <t>complete the scheduled topics</t>
+  </si>
+  <si>
+    <t>give assignments to the trainee</t>
+  </si>
+  <si>
+    <t>evaluate their understandings</t>
+  </si>
+  <si>
+    <t>View the course</t>
+  </si>
+  <si>
+    <t>list of students enrolled</t>
+  </si>
+  <si>
+    <t>View the student list</t>
+  </si>
+  <si>
+    <t>view feedback from the trainee</t>
+  </si>
+  <si>
+    <t>give feedback about the trainee</t>
+  </si>
+  <si>
+    <t>Trainer should have credentials to access the course</t>
+  </si>
+  <si>
+    <t>Trainer should have the trainee</t>
+  </si>
+  <si>
+    <t>Trainer should have a training co-ordinator</t>
+  </si>
+  <si>
+    <t>Trainer should have been allocated to the course</t>
+  </si>
+  <si>
+    <t>Trainer should complete the topics within the scheduled time</t>
+  </si>
+  <si>
+    <t>Trainer can cover all the topics</t>
+  </si>
+  <si>
+    <t>Trainer can give the assignment to the trainees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trainer can give feedback </t>
+  </si>
+  <si>
+    <t>Trainer can view the trainee feedback</t>
+  </si>
+  <si>
+    <t>Acceptance criteria:</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>It should navigate to the assigned course</t>
+  </si>
+  <si>
+    <t>User Story</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a trainer i want to login to the system </t>
+  </si>
+  <si>
+    <t>Can login with the credentials</t>
+  </si>
+  <si>
+    <t>if not you are not allowed to login</t>
+  </si>
+  <si>
+    <t>It should navigate to the Landing Page</t>
   </si>
   <si>
     <t>Landing page is common for all users</t>
-  </si>
-  <si>
-    <t>It should have assigned courses</t>
-  </si>
-  <si>
-    <t>It should view technology,trainer,duration of the assigned courses</t>
-  </si>
-  <si>
-    <t>All course may not be displayed in dashboard</t>
-  </si>
-  <si>
-    <t>It should have scheduled review</t>
-  </si>
-  <si>
-    <t>It should shows review details</t>
-  </si>
-  <si>
-    <t>Review should assigned by  Training cocrdinate</t>
-  </si>
-  <si>
-    <t>It should have search bar</t>
-  </si>
-  <si>
-    <t>It will help the trainee to find the course quickly</t>
-  </si>
-  <si>
-    <t>It should show attendance marking option</t>
-  </si>
-  <si>
-    <t>Trainee has to self mark the attendance status</t>
-  </si>
-  <si>
-    <t>Trainee must be enrolled in that course</t>
-  </si>
-  <si>
-    <t>It should contain topics related to the course</t>
-  </si>
-  <si>
-    <t>It can be video or document materials</t>
-  </si>
-  <si>
-    <t>Topics and  materials updated by trainer</t>
-  </si>
-  <si>
-    <t>It contains trainer assigned</t>
-  </si>
-  <si>
-    <t>It will show the trainer name</t>
-  </si>
-  <si>
-    <t>Trainer should be assigned by  Training coordinate</t>
-  </si>
-  <si>
-    <t>It contains course details</t>
-  </si>
-  <si>
-    <t>It shows (Duration, Course goals, Course description, Prerequisites)</t>
-  </si>
-  <si>
-    <t>Should be created during course  creation</t>
-  </si>
-  <si>
-    <t>It should update attendance</t>
-  </si>
-  <si>
-    <t>It can be check box or dropdown</t>
-  </si>
-  <si>
-    <t>Only for specified time attendence will be available</t>
-  </si>
-  <si>
-    <t>It could be 15-30 mins</t>
-  </si>
-  <si>
-    <t>Trainer can give his views about course and trainer</t>
-  </si>
-  <si>
-    <t>It may be textbox can hold about 500 words</t>
-  </si>
-  <si>
-    <t>The input entered in the textbox should be view by Trainer and coordinator</t>
-  </si>
-  <si>
-    <t>Trainer must be assigned to the course</t>
-  </si>
-  <si>
-    <t>It contains filter option to sort feebacks of specific date</t>
-  </si>
-  <si>
-    <t>It'll get date from the user</t>
-  </si>
-  <si>
-    <t>Date must be valid</t>
-  </si>
-  <si>
-    <t>It can be a grid or list view</t>
-  </si>
-  <si>
-    <t>Activity can be given on daily basis</t>
-  </si>
-  <si>
-    <t>It can be quiz or exploration</t>
-  </si>
-  <si>
-    <t>Activity should be submitted by individual</t>
-  </si>
-  <si>
-    <t>It contains questions as documents</t>
-  </si>
-  <si>
-    <t>trainee can download them</t>
-  </si>
-  <si>
-    <t>current assignment should be completed before the next one</t>
-  </si>
-  <si>
-    <t>Trainee cannot change the deadline</t>
-  </si>
-  <si>
-    <t>Assignments should be submitted before deadline</t>
-  </si>
-  <si>
-    <t>Trainee can upload both pdf and word document</t>
-  </si>
-  <si>
-    <t>Upload document size must be limited</t>
-  </si>
-  <si>
-    <t>It may be overall mark scored or individual course</t>
-  </si>
-  <si>
-    <t>It contains details about the upcoming meeting</t>
-  </si>
-  <si>
-    <t>It should have the meeting link</t>
-  </si>
-  <si>
-    <t>Review must be scheduled by  Training cocrdinate</t>
-  </si>
-  <si>
-    <t>It may have meeting history</t>
-  </si>
-  <si>
-    <t>Review must be completed</t>
-  </si>
-  <si>
-    <t>It contains text fields of Reviewer and date of review</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It may be textbox or dropdown </t>
-  </si>
-  <si>
-    <t xml:space="preserve">It contains fields(actions to be done and meeting notes) </t>
-  </si>
-  <si>
-    <t>MOM must be visible to Training coordinator and reviewer</t>
-  </si>
-  <si>
-    <t>As a trainee i should logout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trainee can logout </t>
-  </si>
-  <si>
-    <t>Redirect to login page</t>
-  </si>
-  <si>
-    <t>internal/external Trainer</t>
-  </si>
-  <si>
-    <t>teach course to the trainees</t>
-  </si>
-  <si>
-    <t>train them properly</t>
-  </si>
-  <si>
-    <t>make them understand the concepts</t>
-  </si>
-  <si>
-    <t>make them gain knowledge</t>
-  </si>
-  <si>
-    <t>plan the schedule</t>
-  </si>
-  <si>
-    <t>complete within the given time</t>
-  </si>
-  <si>
-    <t>guide them with the project</t>
-  </si>
-  <si>
-    <t>Push them for project review</t>
-  </si>
-  <si>
-    <t>conduct a clarification session</t>
-  </si>
-  <si>
-    <t>clarify their doubts</t>
-  </si>
-  <si>
-    <t>Monitor their works</t>
-  </si>
-  <si>
-    <t>know whats their progress</t>
-  </si>
-  <si>
-    <t>track attendence of trainee</t>
-  </si>
-  <si>
-    <t>report to higher ups</t>
-  </si>
-  <si>
-    <t>Provides feedback</t>
-  </si>
-  <si>
-    <t>make trainees improve themself</t>
-  </si>
-  <si>
-    <t>view status Update</t>
-  </si>
-  <si>
-    <t>track them on daily basis</t>
-  </si>
-  <si>
-    <t>Trainer - &gt; Register/Login - &gt;	Attendence - &gt; Plan the Course	- &gt; Assignments - &gt; Session Clarification - &gt; Feedback</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>Trainer</t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Enter into the assigned course</t>
-  </si>
-  <si>
-    <t>View the courses</t>
-  </si>
-  <si>
-    <t>see the course topics</t>
-  </si>
-  <si>
-    <t>View the topics</t>
-  </si>
-  <si>
-    <t>complete the scheduled topics</t>
-  </si>
-  <si>
-    <t>give assignments to the trainee</t>
-  </si>
-  <si>
-    <t>evaluate their understandings</t>
-  </si>
-  <si>
-    <t>View the course</t>
-  </si>
-  <si>
-    <t>list of students enrolled</t>
-  </si>
-  <si>
-    <t>View the student list</t>
-  </si>
-  <si>
-    <t>view feedback from the trainee</t>
-  </si>
-  <si>
-    <t>give feedback about the trainee</t>
-  </si>
-  <si>
-    <t>Trainer should have credentials to access the course</t>
-  </si>
-  <si>
-    <t>Trainer should have the trainee</t>
-  </si>
-  <si>
-    <t>Trainer should have a training co-ordinator</t>
-  </si>
-  <si>
-    <t>Trainer should have been allocated to the course</t>
-  </si>
-  <si>
-    <t>Trainer should complete the topics within the scheduled time</t>
-  </si>
-  <si>
-    <t>Trainer can cover all the topics</t>
-  </si>
-  <si>
-    <t>Trainer can give the assignment to the trainees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trainer can give feedback </t>
-  </si>
-  <si>
-    <t>Trainer can view the trainee feedback</t>
-  </si>
-  <si>
-    <t>Acceptance criteria:</t>
-  </si>
-  <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>It should navigate to the assigned course</t>
-  </si>
-  <si>
-    <t>User Story</t>
-  </si>
-  <si>
-    <t>Acceptance Criteria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a trainer i want to login to the system </t>
-  </si>
-  <si>
-    <t>Can login with the credentials</t>
-  </si>
-  <si>
-    <t>if not you are not allowed to login</t>
-  </si>
-  <si>
-    <t>It should navigate to the Landing Page</t>
   </si>
   <si>
     <t>As a trainer i want to view the  course</t>
@@ -898,6 +933,15 @@
 There should atleast one trainee.</t>
   </si>
   <si>
+    <t>End Of Day 5</t>
+  </si>
+  <si>
+    <t>Training Co-ordinator should have the course Name 
+Training Co-ordinator should have the course Description
+Training Co-ordinator should have the course duration 
+Course should be created and added to the course list.Course list should contain topics.</t>
+  </si>
+  <si>
     <t>Training co-ordinator</t>
   </si>
   <si>
@@ -1223,13 +1267,16 @@
   </si>
   <si>
     <t>https://onedrive.live.com/edit.aspx?resid=87459A6448E6BC93!162&amp;ithint=file%2cxlsx&amp;authkey=!AKifiQlZGxihAuY</t>
+  </si>
+  <si>
+    <t>https://www.figma.com/file/5LtesCL0bdF2ZM1KSsx5QI/TMS?node-id=0%3A1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1382,6 +1429,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1598,7 +1652,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1641,6 +1695,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1734,8 +1791,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -19821,20 +19876,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1066800</xdr:colOff>
-      <xdr:row>301</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2114550</xdr:colOff>
+      <xdr:row>299</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>445</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>443</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="TextBox 2">
+        <xdr:cNvPr id="4" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0FB878C-E557-432A-8308-2DC5F1184F5E}"/>
@@ -19848,8 +19903,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3276600" y="57864375"/>
-          <a:ext cx="32785050" cy="27593925"/>
+          <a:off x="2114550" y="57607200"/>
+          <a:ext cx="35899725" cy="27593925"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -28696,6 +28751,55 @@
         <a:xfrm>
           <a:off x="1962150" y="295275"/>
           <a:ext cx="16992600" cy="7534275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9465DD51-E4AA-CF1E-3E3F-202D30CCD592}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2428875" y="190500"/>
+          <a:ext cx="4791075" cy="4514850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -29094,7 +29198,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U274"/>
+  <dimension ref="A1:U327"/>
   <sheetViews>
     <sheetView topLeftCell="A259" workbookViewId="0">
       <selection activeCell="A273" sqref="A273:E274"/>
@@ -29966,10 +30070,10 @@
     </row>
     <row r="263" spans="1:4">
       <c r="B263" t="s">
-        <v>77</v>
+        <v>135</v>
       </c>
       <c r="C263" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D263" t="s">
         <v>132</v>
@@ -29985,13 +30089,13 @@
     </row>
     <row r="266" spans="1:4">
       <c r="B266" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C266" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D266" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="267" spans="1:4">
@@ -29999,10 +30103,15 @@
         <v>81</v>
       </c>
       <c r="C267" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D267" t="s">
-        <v>140</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4">
+      <c r="B268" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="269" spans="1:4">
@@ -30015,10 +30124,10 @@
     </row>
     <row r="270" spans="1:4">
       <c r="B270" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C270" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D270" t="s">
         <v>123</v>
@@ -30026,29 +30135,399 @@
     </row>
     <row r="271" spans="1:4">
       <c r="B271" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C271" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D271" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="273" spans="1:3">
+    <row r="273" spans="1:4">
       <c r="A273" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B273" s="12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="274" spans="1:3">
+    <row r="274" spans="1:4">
       <c r="B274" t="s">
+        <v>148</v>
+      </c>
+      <c r="C274" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4">
+      <c r="A282" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4">
+      <c r="A283" t="s">
+        <v>87</v>
+      </c>
+      <c r="B283" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C283" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D283" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4">
+      <c r="B284" t="s">
+        <v>88</v>
+      </c>
+      <c r="C284" t="s">
+        <v>51</v>
+      </c>
+      <c r="D284" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4">
+      <c r="B285" t="s">
+        <v>52</v>
+      </c>
+      <c r="C285" t="s">
+        <v>90</v>
+      </c>
+      <c r="D285" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4">
+      <c r="B286" s="44" t="s">
+        <v>150</v>
+      </c>
+      <c r="C286" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="D286" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4">
+      <c r="D287" s="44" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4">
+      <c r="A288" t="s">
+        <v>54</v>
+      </c>
+      <c r="B288" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4">
+      <c r="B289" t="s">
+        <v>93</v>
+      </c>
+      <c r="C289" t="s">
+        <v>94</v>
+      </c>
+      <c r="D289" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4">
+      <c r="B290" t="s">
+        <v>96</v>
+      </c>
+      <c r="C290" t="s">
+        <v>97</v>
+      </c>
+      <c r="D290" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4">
+      <c r="B291" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="C291" s="44" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4">
+      <c r="A293" t="s">
+        <v>58</v>
+      </c>
+      <c r="B293" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4">
+      <c r="B294" t="s">
+        <v>101</v>
+      </c>
+      <c r="C294" t="s">
+        <v>102</v>
+      </c>
+      <c r="D294" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4">
+      <c r="B295" t="s">
+        <v>104</v>
+      </c>
+      <c r="C295" t="s">
+        <v>105</v>
+      </c>
+      <c r="D295" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4">
+      <c r="B296" t="s">
+        <v>153</v>
+      </c>
+      <c r="C296" t="s">
+        <v>108</v>
+      </c>
+      <c r="D296" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4">
+      <c r="B297" t="s">
+        <v>110</v>
+      </c>
+      <c r="C297" t="s">
+        <v>111</v>
+      </c>
+      <c r="D297" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4">
+      <c r="A299" t="s">
+        <v>63</v>
+      </c>
+      <c r="B299" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4">
+      <c r="B300" t="s">
+        <v>154</v>
+      </c>
+      <c r="C300" t="s">
+        <v>114</v>
+      </c>
+      <c r="D300" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4">
+      <c r="B301" t="s">
+        <v>155</v>
+      </c>
+      <c r="C301" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4">
+      <c r="A303" t="s">
+        <v>67</v>
+      </c>
+      <c r="B303" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4">
+      <c r="B304" t="s">
+        <v>156</v>
+      </c>
+      <c r="C304" t="s">
+        <v>118</v>
+      </c>
+      <c r="D304" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4">
+      <c r="B305" t="s">
+        <v>69</v>
+      </c>
+      <c r="C305" t="s">
+        <v>119</v>
+      </c>
+      <c r="D305" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4">
+      <c r="B306" t="s">
+        <v>157</v>
+      </c>
+      <c r="C306" t="s">
+        <v>122</v>
+      </c>
+      <c r="D306" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4">
+      <c r="B307" t="s">
+        <v>70</v>
+      </c>
+      <c r="C307" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4">
+      <c r="A309" t="s">
+        <v>71</v>
+      </c>
+      <c r="B309" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4">
+      <c r="B310" t="s">
+        <v>125</v>
+      </c>
+      <c r="C310" t="s">
+        <v>126</v>
+      </c>
+      <c r="D310" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4">
+      <c r="B311" t="s">
+        <v>128</v>
+      </c>
+      <c r="C311" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D311" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4">
+      <c r="B312" t="s">
+        <v>74</v>
+      </c>
+      <c r="C312" t="s">
+        <v>131</v>
+      </c>
+      <c r="D312" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4">
+      <c r="A314" t="s">
+        <v>75</v>
+      </c>
+      <c r="B314" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4">
+      <c r="B315" t="s">
+        <v>76</v>
+      </c>
+      <c r="C315" t="s">
+        <v>133</v>
+      </c>
+      <c r="D315" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4">
+      <c r="B316" t="s">
+        <v>77</v>
+      </c>
+      <c r="C316" t="s">
+        <v>136</v>
+      </c>
+      <c r="D316" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4">
+      <c r="A318" t="s">
+        <v>78</v>
+      </c>
+      <c r="B318" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4">
+      <c r="B319" t="s">
+        <v>137</v>
+      </c>
+      <c r="C319" t="s">
+        <v>138</v>
+      </c>
+      <c r="D319" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4">
+      <c r="B320" t="s">
+        <v>81</v>
+      </c>
+      <c r="C320" t="s">
+        <v>140</v>
+      </c>
+      <c r="D320" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4">
+      <c r="A322" t="s">
+        <v>82</v>
+      </c>
+      <c r="B322" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4">
+      <c r="B323" t="s">
+        <v>143</v>
+      </c>
+      <c r="C323" t="s">
+        <v>144</v>
+      </c>
+      <c r="D323" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4">
+      <c r="B324" t="s">
+        <v>145</v>
+      </c>
+      <c r="C324" t="s">
         <v>146</v>
       </c>
-      <c r="C274" s="5" t="s">
+      <c r="D324" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4">
+      <c r="A326" t="s">
         <v>147</v>
+      </c>
+      <c r="B326" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4">
+      <c r="B327" t="s">
+        <v>148</v>
+      </c>
+      <c r="C327" s="5" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -30060,12 +30539,33 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A40FD46-800B-461D-A3BD-D88C30A95649}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="25" t="s">
+        <v>402</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{2158389B-7B96-4D6A-B0AB-2968BC422701}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A29A159-1DDF-4514-8C0F-74BD61563D65}">
   <dimension ref="A3:U208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="A197" sqref="A197:XFD197"/>
+    <sheetView topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="A197" sqref="A197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30097,13 +30597,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C5" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="D5" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -30111,13 +30611,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C6" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="D6" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -30125,13 +30625,13 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C7" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="D7" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -30139,13 +30639,13 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C8" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="D8" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -30153,13 +30653,13 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C9" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="D9" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -30167,13 +30667,13 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C10" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="D10" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -30181,13 +30681,13 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C11" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="D11" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -30195,13 +30695,13 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C12" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="D12" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -30209,13 +30709,13 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C13" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="D13" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -30223,7 +30723,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
@@ -30239,7 +30739,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="B19" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="27" customHeight="1">
@@ -30289,7 +30789,7 @@
     </row>
     <row r="62" spans="10:10">
       <c r="J62" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="74" spans="2:5" ht="18.75">
@@ -30311,61 +30811,61 @@
         <v>1</v>
       </c>
       <c r="C75" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="D75" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="E75" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
     </row>
     <row r="76" spans="2:5">
       <c r="D76" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="E76" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
     </row>
     <row r="77" spans="2:5">
       <c r="D77" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="E77" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
     </row>
     <row r="78" spans="2:5">
       <c r="D78" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="E78" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
     </row>
     <row r="80" spans="2:5">
       <c r="D80" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="E80" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
     </row>
     <row r="81" spans="4:5">
       <c r="D81" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="E81" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
     </row>
     <row r="82" spans="4:5">
       <c r="D82" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="E82" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
     </row>
     <row r="119" spans="1:15" ht="33" customHeight="1">
@@ -30411,27 +30911,27 @@
     </row>
     <row r="125" spans="1:15">
       <c r="A125" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
     </row>
     <row r="126" spans="1:15">
       <c r="A126" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
     </row>
     <row r="127" spans="1:15">
       <c r="A127" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
     </row>
     <row r="128" spans="1:15">
       <c r="A128" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="26.25">
@@ -30441,27 +30941,27 @@
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="C144" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -30476,15 +30976,15 @@
     </row>
     <row r="148" spans="1:4">
       <c r="B148" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="D148" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="21">
       <c r="A153" s="4" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="21">
@@ -30519,10 +31019,10 @@
     </row>
     <row r="188" spans="1:21">
       <c r="A188" s="12" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="B188" s="12" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="C188" s="12" t="s">
         <v>35</v>
@@ -30532,220 +31032,220 @@
       </c>
     </row>
     <row r="189" spans="1:21" ht="15.75">
-      <c r="A189" s="73"/>
-      <c r="B189" s="73"/>
-      <c r="C189" s="73"/>
-      <c r="D189" s="73"/>
-      <c r="E189" s="73"/>
+      <c r="A189" s="42"/>
+      <c r="B189" s="42"/>
+      <c r="C189" s="42"/>
+      <c r="D189" s="42"/>
+      <c r="E189" s="42"/>
     </row>
     <row r="190" spans="1:21" ht="15.75">
-      <c r="A190" s="73" t="s">
-        <v>197</v>
-      </c>
-      <c r="B190" s="73" t="s">
+      <c r="A190" s="42" t="s">
+        <v>207</v>
+      </c>
+      <c r="B190" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="C190" s="73" t="s">
-        <v>198</v>
-      </c>
-      <c r="D190" s="73" t="s">
+      <c r="C190" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="D190" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="E190" s="73"/>
+      <c r="E190" s="42"/>
     </row>
     <row r="191" spans="1:21" ht="15.75">
-      <c r="A191" s="73"/>
-      <c r="B191" s="73" t="s">
+      <c r="A191" s="42"/>
+      <c r="B191" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="C191" s="73" t="s">
-        <v>199</v>
-      </c>
-      <c r="D191" s="73" t="s">
+      <c r="C191" s="42" t="s">
+        <v>209</v>
+      </c>
+      <c r="D191" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="E191" s="73"/>
+      <c r="E191" s="42"/>
     </row>
     <row r="192" spans="1:21" ht="15.75">
-      <c r="A192" s="73"/>
-      <c r="B192" s="73" t="s">
-        <v>200</v>
-      </c>
-      <c r="C192" s="73" t="s">
-        <v>92</v>
-      </c>
-      <c r="D192" s="73" t="s">
+      <c r="A192" s="42"/>
+      <c r="B192" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="C192" s="42" t="s">
+        <v>211</v>
+      </c>
+      <c r="D192" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="E192" s="73"/>
+      <c r="E192" s="42"/>
     </row>
     <row r="193" spans="1:5" ht="15.75">
-      <c r="A193" s="73"/>
-      <c r="B193" s="73"/>
-      <c r="C193" s="73"/>
-      <c r="D193" s="73"/>
-      <c r="E193" s="73"/>
+      <c r="A193" s="42"/>
+      <c r="B193" s="42"/>
+      <c r="C193" s="42"/>
+      <c r="D193" s="42"/>
+      <c r="E193" s="42"/>
     </row>
     <row r="194" spans="1:5" ht="15.75">
-      <c r="A194" s="73" t="s">
-        <v>201</v>
-      </c>
-      <c r="B194" s="73" t="s">
-        <v>202</v>
-      </c>
-      <c r="C194" s="73" t="s">
-        <v>203</v>
-      </c>
-      <c r="D194" s="73" t="s">
-        <v>204</v>
-      </c>
-      <c r="E194" s="73"/>
+      <c r="A194" s="42" t="s">
+        <v>212</v>
+      </c>
+      <c r="B194" s="42" t="s">
+        <v>213</v>
+      </c>
+      <c r="C194" s="42" t="s">
+        <v>214</v>
+      </c>
+      <c r="D194" s="42" t="s">
+        <v>215</v>
+      </c>
+      <c r="E194" s="42"/>
     </row>
     <row r="195" spans="1:5" ht="15.75">
-      <c r="A195" s="73"/>
-      <c r="B195" s="73" t="s">
+      <c r="A195" s="42"/>
+      <c r="B195" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="C195" s="73" t="s">
-        <v>205</v>
-      </c>
-      <c r="D195" s="73" t="s">
-        <v>206</v>
-      </c>
-      <c r="E195" s="73"/>
+      <c r="C195" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="D195" s="42" t="s">
+        <v>217</v>
+      </c>
+      <c r="E195" s="42"/>
     </row>
     <row r="196" spans="1:5" ht="15.75">
-      <c r="A196" s="73"/>
-      <c r="B196" s="73"/>
-      <c r="C196" s="73"/>
-      <c r="D196" s="73"/>
-      <c r="E196" s="73"/>
+      <c r="A196" s="42"/>
+      <c r="B196" s="42"/>
+      <c r="C196" s="42"/>
+      <c r="D196" s="42"/>
+      <c r="E196" s="42"/>
     </row>
     <row r="197" spans="1:5" ht="15.75">
-      <c r="A197" s="73"/>
-      <c r="B197" s="73"/>
-      <c r="C197" s="73"/>
-      <c r="D197" s="73"/>
-      <c r="E197" s="73"/>
+      <c r="A197" s="42"/>
+      <c r="B197" s="42"/>
+      <c r="C197" s="42"/>
+      <c r="D197" s="42"/>
+      <c r="E197" s="42"/>
     </row>
     <row r="198" spans="1:5" ht="15.75">
-      <c r="A198" s="74" t="s">
-        <v>207</v>
-      </c>
-      <c r="B198" s="73" t="s">
-        <v>208</v>
-      </c>
-      <c r="C198" s="73" t="s">
-        <v>203</v>
-      </c>
-      <c r="D198" s="73" t="s">
-        <v>209</v>
-      </c>
-      <c r="E198" s="73"/>
+      <c r="A198" s="43" t="s">
+        <v>218</v>
+      </c>
+      <c r="B198" s="42" t="s">
+        <v>219</v>
+      </c>
+      <c r="C198" s="42" t="s">
+        <v>214</v>
+      </c>
+      <c r="D198" s="42" t="s">
+        <v>220</v>
+      </c>
+      <c r="E198" s="42"/>
     </row>
     <row r="199" spans="1:5" ht="15.75">
-      <c r="A199" s="73"/>
-      <c r="B199" s="73" t="s">
-        <v>210</v>
-      </c>
-      <c r="C199" s="73" t="s">
-        <v>211</v>
-      </c>
-      <c r="D199" s="73" t="s">
-        <v>212</v>
-      </c>
-      <c r="E199" s="73"/>
+      <c r="A199" s="42"/>
+      <c r="B199" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="C199" s="42" t="s">
+        <v>222</v>
+      </c>
+      <c r="D199" s="42" t="s">
+        <v>223</v>
+      </c>
+      <c r="E199" s="42"/>
     </row>
     <row r="200" spans="1:5" ht="15.75">
-      <c r="A200" s="73"/>
-      <c r="B200" s="73"/>
-      <c r="C200" s="73"/>
-      <c r="D200" s="73"/>
-      <c r="E200" s="73"/>
+      <c r="A200" s="42"/>
+      <c r="B200" s="42"/>
+      <c r="C200" s="42"/>
+      <c r="D200" s="42"/>
+      <c r="E200" s="42"/>
     </row>
     <row r="201" spans="1:5" ht="15.75">
-      <c r="A201" s="73"/>
-      <c r="B201" s="73"/>
-      <c r="C201" s="73"/>
-      <c r="D201" s="73"/>
-      <c r="E201" s="73"/>
+      <c r="A201" s="42"/>
+      <c r="B201" s="42"/>
+      <c r="C201" s="42"/>
+      <c r="D201" s="42"/>
+      <c r="E201" s="42"/>
     </row>
     <row r="202" spans="1:5" ht="15.75">
-      <c r="A202" s="73" t="s">
-        <v>213</v>
-      </c>
-      <c r="B202" s="73" t="s">
-        <v>214</v>
-      </c>
-      <c r="C202" s="73" t="s">
-        <v>215</v>
-      </c>
-      <c r="D202" s="73" t="s">
+      <c r="A202" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="B202" s="42" t="s">
+        <v>225</v>
+      </c>
+      <c r="C202" s="42" t="s">
+        <v>226</v>
+      </c>
+      <c r="D202" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="E202" s="73"/>
+      <c r="E202" s="42"/>
     </row>
     <row r="203" spans="1:5" ht="15.75">
-      <c r="A203" s="73"/>
-      <c r="B203" s="73" t="s">
-        <v>216</v>
-      </c>
-      <c r="C203" s="73" t="s">
-        <v>217</v>
-      </c>
-      <c r="D203" s="73" t="s">
-        <v>218</v>
-      </c>
-      <c r="E203" s="73"/>
+      <c r="A203" s="42"/>
+      <c r="B203" s="42" t="s">
+        <v>227</v>
+      </c>
+      <c r="C203" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="D203" s="42" t="s">
+        <v>229</v>
+      </c>
+      <c r="E203" s="42"/>
     </row>
     <row r="204" spans="1:5" ht="15.75">
-      <c r="A204" s="73"/>
-      <c r="B204" s="73"/>
-      <c r="C204" s="73"/>
-      <c r="D204" s="73"/>
-      <c r="E204" s="73"/>
+      <c r="A204" s="42"/>
+      <c r="B204" s="42"/>
+      <c r="C204" s="42"/>
+      <c r="D204" s="42"/>
+      <c r="E204" s="42"/>
     </row>
     <row r="205" spans="1:5" ht="15.75">
-      <c r="A205" s="73"/>
-      <c r="B205" s="73"/>
-      <c r="C205" s="73"/>
-      <c r="D205" s="73"/>
-      <c r="E205" s="73"/>
+      <c r="A205" s="42"/>
+      <c r="B205" s="42"/>
+      <c r="C205" s="42"/>
+      <c r="D205" s="42"/>
+      <c r="E205" s="42"/>
     </row>
     <row r="206" spans="1:5" ht="15.75">
-      <c r="A206" s="73" t="s">
-        <v>219</v>
-      </c>
-      <c r="B206" s="73" t="s">
-        <v>220</v>
-      </c>
-      <c r="C206" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="D206" s="73" t="s">
-        <v>222</v>
-      </c>
-      <c r="E206" s="73"/>
+      <c r="A206" s="42" t="s">
+        <v>230</v>
+      </c>
+      <c r="B206" s="42" t="s">
+        <v>231</v>
+      </c>
+      <c r="C206" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="D206" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="E206" s="42"/>
     </row>
     <row r="207" spans="1:5" ht="15.75">
-      <c r="A207" s="73"/>
-      <c r="B207" s="73"/>
-      <c r="C207" s="73"/>
-      <c r="D207" s="73"/>
-      <c r="E207" s="73"/>
+      <c r="A207" s="42"/>
+      <c r="B207" s="42"/>
+      <c r="C207" s="42"/>
+      <c r="D207" s="42"/>
+      <c r="E207" s="42"/>
     </row>
     <row r="208" spans="1:5">
       <c r="A208" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B208" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
       <c r="C208" s="5" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D208" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -30761,9 +31261,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D891E2A-7FE3-4EFF-91F2-3D1BB267DA87}">
-  <dimension ref="A2:S585"/>
+  <dimension ref="A2:T585"/>
   <sheetViews>
-    <sheetView topLeftCell="D452" workbookViewId="0">
+    <sheetView topLeftCell="D451" workbookViewId="0">
       <selection activeCell="E462" sqref="E462:E466"/>
     </sheetView>
   </sheetViews>
@@ -30772,9 +31272,10 @@
     <col min="1" max="1" width="33.140625" customWidth="1"/>
     <col min="2" max="2" width="50.5703125" customWidth="1"/>
     <col min="3" max="3" width="119" customWidth="1"/>
-    <col min="4" max="4" width="85" customWidth="1"/>
+    <col min="4" max="4" width="105.140625" customWidth="1"/>
     <col min="5" max="5" width="81.5703125" customWidth="1"/>
     <col min="6" max="6" width="51" customWidth="1"/>
+    <col min="7" max="7" width="52" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="18.75">
@@ -30796,13 +31297,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="C3" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="D3" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -30810,13 +31311,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="C4" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="D4" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -30824,13 +31325,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="C5" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="D5" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -30838,13 +31339,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="C6" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="D6" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -30852,13 +31353,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="C7" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="D7" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -30866,13 +31367,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="C8" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="D8" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -30880,13 +31381,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="C9" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="D9" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -30894,13 +31395,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="C10" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
       <c r="D10" t="s">
-        <v>241</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -30908,13 +31409,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="C11" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="D11" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -30922,13 +31423,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="C12" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="D12" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -30936,13 +31437,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="C13" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="D13" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="18.75">
@@ -30954,7 +31455,7 @@
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="9" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -30982,13 +31483,13 @@
     </row>
     <row r="120" spans="5:5">
       <c r="E120" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
     </row>
     <row r="160" spans="1:18" ht="36.75" customHeight="1">
       <c r="A160" s="16"/>
       <c r="B160" s="16" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="C160" s="19" t="s">
         <v>33</v>
@@ -31035,7 +31536,7 @@
     <row r="449" spans="2:19" ht="33.75">
       <c r="B449" s="16"/>
       <c r="C449" s="16" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="D449" s="19" t="s">
         <v>85</v>
@@ -31078,10 +31579,10 @@
     </row>
     <row r="457" spans="2:19">
       <c r="C457" s="28" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="D457" s="28" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="E457" s="28" t="s">
         <v>35</v>
@@ -31091,361 +31592,699 @@
       </c>
     </row>
     <row r="458" spans="2:19" ht="25.5" customHeight="1">
-      <c r="C458" s="48" t="s">
-        <v>251</v>
-      </c>
-      <c r="D458" s="52" t="s">
-        <v>252</v>
-      </c>
-      <c r="E458" s="58"/>
-      <c r="F458" s="49" t="s">
-        <v>253</v>
+      <c r="C458" s="51" t="s">
+        <v>262</v>
+      </c>
+      <c r="D458" s="55" t="s">
+        <v>263</v>
+      </c>
+      <c r="E458" s="61"/>
+      <c r="F458" s="52" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="459" spans="2:19" ht="18.75" customHeight="1">
-      <c r="C459" s="43"/>
-      <c r="D459" s="53"/>
-      <c r="E459" s="59"/>
-      <c r="F459" s="50"/>
+      <c r="C459" s="46"/>
+      <c r="D459" s="56"/>
+      <c r="E459" s="62"/>
+      <c r="F459" s="53"/>
     </row>
     <row r="460" spans="2:19">
-      <c r="C460" s="43"/>
-      <c r="D460" s="53"/>
-      <c r="E460" s="59"/>
-      <c r="F460" s="50"/>
+      <c r="C460" s="46"/>
+      <c r="D460" s="56"/>
+      <c r="E460" s="62"/>
+      <c r="F460" s="53"/>
     </row>
     <row r="461" spans="2:19">
-      <c r="C461" s="44"/>
-      <c r="D461" s="54"/>
-      <c r="E461" s="60"/>
-      <c r="F461" s="50"/>
+      <c r="C461" s="47"/>
+      <c r="D461" s="57"/>
+      <c r="E461" s="63"/>
+      <c r="F461" s="53"/>
     </row>
     <row r="462" spans="2:19" ht="15" customHeight="1">
-      <c r="C462" s="48" t="s">
-        <v>254</v>
-      </c>
-      <c r="D462" s="42" t="s">
-        <v>255</v>
-      </c>
-      <c r="E462" s="65" t="s">
-        <v>256</v>
-      </c>
-      <c r="F462" s="48" t="s">
-        <v>257</v>
+      <c r="C462" s="51" t="s">
+        <v>265</v>
+      </c>
+      <c r="D462" s="45" t="s">
+        <v>266</v>
+      </c>
+      <c r="E462" s="68" t="s">
+        <v>267</v>
+      </c>
+      <c r="F462" s="51" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="463" spans="2:19">
-      <c r="C463" s="43"/>
-      <c r="D463" s="45"/>
-      <c r="E463" s="66"/>
-      <c r="F463" s="43"/>
+      <c r="C463" s="46"/>
+      <c r="D463" s="48"/>
+      <c r="E463" s="69"/>
+      <c r="F463" s="46"/>
     </row>
     <row r="464" spans="2:19">
-      <c r="C464" s="43"/>
-      <c r="D464" s="45"/>
-      <c r="E464" s="66"/>
-      <c r="F464" s="43"/>
+      <c r="C464" s="46"/>
+      <c r="D464" s="48"/>
+      <c r="E464" s="69"/>
+      <c r="F464" s="46"/>
     </row>
     <row r="465" spans="3:6">
-      <c r="C465" s="43"/>
-      <c r="D465" s="45"/>
-      <c r="E465" s="66"/>
-      <c r="F465" s="43"/>
+      <c r="C465" s="46"/>
+      <c r="D465" s="48"/>
+      <c r="E465" s="69"/>
+      <c r="F465" s="46"/>
     </row>
     <row r="466" spans="3:6">
-      <c r="C466" s="44"/>
-      <c r="D466" s="46"/>
-      <c r="E466" s="67"/>
-      <c r="F466" s="44"/>
+      <c r="C466" s="47"/>
+      <c r="D466" s="49"/>
+      <c r="E466" s="70"/>
+      <c r="F466" s="47"/>
     </row>
     <row r="467" spans="3:6">
-      <c r="C467" s="48" t="s">
-        <v>258</v>
-      </c>
-      <c r="D467" s="47" t="s">
-        <v>255</v>
-      </c>
-      <c r="E467" s="70" t="s">
-        <v>259</v>
-      </c>
-      <c r="F467" s="43" t="s">
-        <v>260</v>
+      <c r="C467" s="51" t="s">
+        <v>269</v>
+      </c>
+      <c r="D467" s="50" t="s">
+        <v>266</v>
+      </c>
+      <c r="E467" s="73" t="s">
+        <v>270</v>
+      </c>
+      <c r="F467" s="46" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="468" spans="3:6">
-      <c r="C468" s="43"/>
-      <c r="D468" s="75"/>
-      <c r="E468" s="71"/>
-      <c r="F468" s="43"/>
+      <c r="C468" s="46"/>
+      <c r="D468" s="76"/>
+      <c r="E468" s="74"/>
+      <c r="F468" s="46"/>
     </row>
     <row r="469" spans="3:6">
-      <c r="C469" s="44"/>
-      <c r="D469" s="75"/>
-      <c r="E469" s="72"/>
-      <c r="F469" s="44"/>
+      <c r="C469" s="47"/>
+      <c r="D469" s="76"/>
+      <c r="E469" s="75"/>
+      <c r="F469" s="47"/>
     </row>
     <row r="470" spans="3:6">
-      <c r="C470" s="48" t="s">
-        <v>261</v>
-      </c>
-      <c r="D470" s="42" t="s">
-        <v>262</v>
-      </c>
-      <c r="E470" s="48"/>
-      <c r="F470" s="55" t="s">
-        <v>263</v>
+      <c r="C470" s="51" t="s">
+        <v>272</v>
+      </c>
+      <c r="D470" s="45" t="s">
+        <v>273</v>
+      </c>
+      <c r="E470" s="51"/>
+      <c r="F470" s="58" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="471" spans="3:6">
-      <c r="C471" s="43"/>
-      <c r="D471" s="43"/>
-      <c r="E471" s="43"/>
-      <c r="F471" s="68"/>
+      <c r="C471" s="46"/>
+      <c r="D471" s="46"/>
+      <c r="E471" s="46"/>
+      <c r="F471" s="71"/>
     </row>
     <row r="472" spans="3:6">
-      <c r="C472" s="43"/>
-      <c r="D472" s="43"/>
-      <c r="E472" s="43"/>
-      <c r="F472" s="68"/>
+      <c r="C472" s="46"/>
+      <c r="D472" s="46"/>
+      <c r="E472" s="46"/>
+      <c r="F472" s="71"/>
     </row>
     <row r="473" spans="3:6">
-      <c r="C473" s="43"/>
-      <c r="D473" s="43"/>
-      <c r="E473" s="43"/>
-      <c r="F473" s="68"/>
+      <c r="C473" s="46"/>
+      <c r="D473" s="46"/>
+      <c r="E473" s="46"/>
+      <c r="F473" s="71"/>
     </row>
     <row r="474" spans="3:6">
-      <c r="C474" s="44"/>
-      <c r="D474" s="44"/>
-      <c r="E474" s="44"/>
-      <c r="F474" s="69"/>
+      <c r="C474" s="47"/>
+      <c r="D474" s="47"/>
+      <c r="E474" s="47"/>
+      <c r="F474" s="72"/>
     </row>
     <row r="475" spans="3:6">
-      <c r="C475" s="48" t="s">
-        <v>264</v>
-      </c>
-      <c r="D475" s="55" t="s">
-        <v>265</v>
-      </c>
-      <c r="E475" s="61"/>
-      <c r="F475" s="55" t="s">
-        <v>266</v>
+      <c r="C475" s="51" t="s">
+        <v>275</v>
+      </c>
+      <c r="D475" s="58" t="s">
+        <v>276</v>
+      </c>
+      <c r="E475" s="64"/>
+      <c r="F475" s="58" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="476" spans="3:6">
-      <c r="C476" s="43"/>
-      <c r="D476" s="56"/>
-      <c r="E476" s="62"/>
-      <c r="F476" s="68"/>
+      <c r="C476" s="46"/>
+      <c r="D476" s="59"/>
+      <c r="E476" s="65"/>
+      <c r="F476" s="71"/>
     </row>
     <row r="477" spans="3:6">
-      <c r="C477" s="43"/>
-      <c r="D477" s="56"/>
-      <c r="E477" s="62"/>
-      <c r="F477" s="68"/>
+      <c r="C477" s="46"/>
+      <c r="D477" s="59"/>
+      <c r="E477" s="65"/>
+      <c r="F477" s="71"/>
     </row>
     <row r="478" spans="3:6">
-      <c r="C478" s="43"/>
-      <c r="D478" s="56"/>
-      <c r="E478" s="62"/>
-      <c r="F478" s="68"/>
+      <c r="C478" s="46"/>
+      <c r="D478" s="59"/>
+      <c r="E478" s="65"/>
+      <c r="F478" s="71"/>
     </row>
     <row r="479" spans="3:6">
-      <c r="C479" s="44"/>
-      <c r="D479" s="57"/>
-      <c r="E479" s="63"/>
-      <c r="F479" s="69"/>
+      <c r="C479" s="47"/>
+      <c r="D479" s="60"/>
+      <c r="E479" s="66"/>
+      <c r="F479" s="72"/>
     </row>
     <row r="480" spans="3:6">
-      <c r="C480" s="43" t="s">
-        <v>267</v>
-      </c>
-      <c r="D480" s="52" t="s">
-        <v>265</v>
-      </c>
-      <c r="E480" s="58"/>
-      <c r="F480" s="55" t="s">
-        <v>268</v>
+      <c r="C480" s="46" t="s">
+        <v>278</v>
+      </c>
+      <c r="D480" s="55" t="s">
+        <v>276</v>
+      </c>
+      <c r="E480" s="61"/>
+      <c r="F480" s="58" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="481" spans="2:6">
-      <c r="C481" s="43"/>
-      <c r="D481" s="53"/>
-      <c r="E481" s="59"/>
-      <c r="F481" s="56"/>
+      <c r="C481" s="46"/>
+      <c r="D481" s="56"/>
+      <c r="E481" s="62"/>
+      <c r="F481" s="59"/>
     </row>
     <row r="482" spans="2:6">
-      <c r="C482" s="43"/>
-      <c r="D482" s="53"/>
-      <c r="E482" s="59"/>
-      <c r="F482" s="56"/>
+      <c r="C482" s="46"/>
+      <c r="D482" s="56"/>
+      <c r="E482" s="62"/>
+      <c r="F482" s="59"/>
     </row>
     <row r="483" spans="2:6">
-      <c r="C483" s="44"/>
-      <c r="D483" s="54"/>
-      <c r="E483" s="60"/>
-      <c r="F483" s="57"/>
+      <c r="C483" s="47"/>
+      <c r="D483" s="57"/>
+      <c r="E483" s="63"/>
+      <c r="F483" s="60"/>
     </row>
     <row r="484" spans="2:6">
-      <c r="C484" s="48" t="s">
-        <v>269</v>
-      </c>
-      <c r="D484" s="52" t="s">
-        <v>270</v>
-      </c>
-      <c r="E484" s="55" t="s">
-        <v>271</v>
-      </c>
-      <c r="F484" s="55" t="s">
-        <v>272</v>
+      <c r="C484" s="51" t="s">
+        <v>280</v>
+      </c>
+      <c r="D484" s="55" t="s">
+        <v>281</v>
+      </c>
+      <c r="E484" s="58" t="s">
+        <v>282</v>
+      </c>
+      <c r="F484" s="58" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="485" spans="2:6" ht="17.25" customHeight="1">
       <c r="B485" s="20"/>
-      <c r="C485" s="43"/>
-      <c r="D485" s="53"/>
-      <c r="E485" s="68"/>
-      <c r="F485" s="68"/>
+      <c r="C485" s="46"/>
+      <c r="D485" s="56"/>
+      <c r="E485" s="71"/>
+      <c r="F485" s="71"/>
     </row>
     <row r="486" spans="2:6">
-      <c r="C486" s="43"/>
-      <c r="D486" s="53"/>
-      <c r="E486" s="68"/>
-      <c r="F486" s="68"/>
+      <c r="C486" s="46"/>
+      <c r="D486" s="56"/>
+      <c r="E486" s="71"/>
+      <c r="F486" s="71"/>
     </row>
     <row r="487" spans="2:6">
-      <c r="C487" s="44"/>
-      <c r="D487" s="54"/>
-      <c r="E487" s="69"/>
-      <c r="F487" s="69"/>
+      <c r="C487" s="47"/>
+      <c r="D487" s="57"/>
+      <c r="E487" s="72"/>
+      <c r="F487" s="72"/>
     </row>
     <row r="488" spans="2:6">
-      <c r="C488" s="48" t="s">
-        <v>273</v>
-      </c>
-      <c r="D488" s="49" t="s">
-        <v>274</v>
-      </c>
-      <c r="E488" s="58"/>
-      <c r="F488" s="55" t="s">
-        <v>275</v>
+      <c r="C488" s="51" t="s">
+        <v>284</v>
+      </c>
+      <c r="D488" s="52" t="s">
+        <v>285</v>
+      </c>
+      <c r="E488" s="61"/>
+      <c r="F488" s="58" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="489" spans="2:6">
-      <c r="C489" s="43"/>
-      <c r="D489" s="50"/>
-      <c r="E489" s="59"/>
-      <c r="F489" s="68"/>
+      <c r="C489" s="46"/>
+      <c r="D489" s="53"/>
+      <c r="E489" s="62"/>
+      <c r="F489" s="71"/>
     </row>
     <row r="490" spans="2:6">
-      <c r="C490" s="43"/>
-      <c r="D490" s="50"/>
-      <c r="E490" s="59"/>
-      <c r="F490" s="68"/>
+      <c r="C490" s="46"/>
+      <c r="D490" s="53"/>
+      <c r="E490" s="62"/>
+      <c r="F490" s="71"/>
     </row>
     <row r="491" spans="2:6">
-      <c r="C491" s="44"/>
-      <c r="D491" s="51"/>
-      <c r="E491" s="60"/>
-      <c r="F491" s="69"/>
+      <c r="C491" s="47"/>
+      <c r="D491" s="54"/>
+      <c r="E491" s="63"/>
+      <c r="F491" s="72"/>
     </row>
     <row r="492" spans="2:6">
-      <c r="C492" s="48" t="s">
-        <v>276</v>
-      </c>
-      <c r="D492" s="52" t="s">
-        <v>277</v>
-      </c>
-      <c r="E492" s="64" t="s">
-        <v>278</v>
-      </c>
-      <c r="F492" s="55" t="s">
-        <v>279</v>
+      <c r="C492" s="51" t="s">
+        <v>287</v>
+      </c>
+      <c r="D492" s="55" t="s">
+        <v>288</v>
+      </c>
+      <c r="E492" s="67" t="s">
+        <v>289</v>
+      </c>
+      <c r="F492" s="58" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="493" spans="2:6">
-      <c r="C493" s="43"/>
-      <c r="D493" s="53"/>
-      <c r="E493" s="56"/>
-      <c r="F493" s="56"/>
+      <c r="C493" s="46"/>
+      <c r="D493" s="56"/>
+      <c r="E493" s="59"/>
+      <c r="F493" s="59"/>
     </row>
     <row r="494" spans="2:6">
-      <c r="C494" s="43"/>
-      <c r="D494" s="53"/>
-      <c r="E494" s="56"/>
-      <c r="F494" s="56"/>
+      <c r="C494" s="46"/>
+      <c r="D494" s="56"/>
+      <c r="E494" s="59"/>
+      <c r="F494" s="59"/>
     </row>
     <row r="495" spans="2:6" ht="16.5" customHeight="1">
       <c r="B495" s="20"/>
-      <c r="C495" s="44"/>
-      <c r="D495" s="54"/>
-      <c r="E495" s="57"/>
-      <c r="F495" s="57"/>
-    </row>
-    <row r="538" spans="1:2" ht="26.25">
+      <c r="C495" s="47"/>
+      <c r="D495" s="57"/>
+      <c r="E495" s="60"/>
+      <c r="F495" s="60"/>
+    </row>
+    <row r="501" spans="3:20" ht="33.75">
+      <c r="C501" s="16"/>
+      <c r="D501" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="E501" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="F501" s="16"/>
+      <c r="G501" s="17"/>
+      <c r="H501" s="16"/>
+      <c r="I501" s="16"/>
+      <c r="J501" s="16"/>
+      <c r="K501" s="16"/>
+      <c r="L501" s="16"/>
+      <c r="M501" s="16"/>
+      <c r="N501" s="16"/>
+      <c r="O501" s="16"/>
+      <c r="P501" s="16"/>
+      <c r="Q501" s="16"/>
+      <c r="R501" s="16"/>
+      <c r="S501" s="16"/>
+      <c r="T501" s="16"/>
+    </row>
+    <row r="502" spans="3:20">
+      <c r="C502" s="16"/>
+      <c r="D502" s="16"/>
+      <c r="E502" s="16"/>
+      <c r="F502" s="16"/>
+      <c r="G502" s="16"/>
+      <c r="H502" s="16"/>
+      <c r="I502" s="16"/>
+      <c r="J502" s="16"/>
+      <c r="K502" s="16"/>
+      <c r="L502" s="16"/>
+      <c r="M502" s="16"/>
+      <c r="N502" s="16"/>
+      <c r="O502" s="16"/>
+      <c r="P502" s="16"/>
+      <c r="Q502" s="16"/>
+      <c r="R502" s="16"/>
+      <c r="S502" s="16"/>
+      <c r="T502" s="16"/>
+    </row>
+    <row r="508" spans="3:20">
+      <c r="D508" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="E508" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="F508" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G508" s="28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="509" spans="3:20">
+      <c r="D509" s="51" t="s">
+        <v>262</v>
+      </c>
+      <c r="E509" s="55" t="s">
+        <v>263</v>
+      </c>
+      <c r="F509" s="61"/>
+      <c r="G509" s="52" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="510" spans="3:20">
+      <c r="D510" s="46"/>
+      <c r="E510" s="56"/>
+      <c r="F510" s="62"/>
+      <c r="G510" s="53"/>
+    </row>
+    <row r="511" spans="3:20">
+      <c r="D511" s="46"/>
+      <c r="E511" s="56"/>
+      <c r="F511" s="62"/>
+      <c r="G511" s="53"/>
+    </row>
+    <row r="512" spans="3:20">
+      <c r="D512" s="47"/>
+      <c r="E512" s="57"/>
+      <c r="F512" s="63"/>
+      <c r="G512" s="53"/>
+    </row>
+    <row r="513" spans="4:7">
+      <c r="D513" s="51" t="s">
+        <v>265</v>
+      </c>
+      <c r="E513" s="45" t="s">
+        <v>266</v>
+      </c>
+      <c r="F513" s="68" t="s">
+        <v>267</v>
+      </c>
+      <c r="G513" s="51" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="514" spans="4:7">
+      <c r="D514" s="46"/>
+      <c r="E514" s="48"/>
+      <c r="F514" s="69"/>
+      <c r="G514" s="46"/>
+    </row>
+    <row r="515" spans="4:7">
+      <c r="D515" s="46"/>
+      <c r="E515" s="48"/>
+      <c r="F515" s="69"/>
+      <c r="G515" s="46"/>
+    </row>
+    <row r="516" spans="4:7">
+      <c r="D516" s="46"/>
+      <c r="E516" s="48"/>
+      <c r="F516" s="69"/>
+      <c r="G516" s="46"/>
+    </row>
+    <row r="517" spans="4:7">
+      <c r="D517" s="47"/>
+      <c r="E517" s="49"/>
+      <c r="F517" s="70"/>
+      <c r="G517" s="47"/>
+    </row>
+    <row r="518" spans="4:7">
+      <c r="D518" s="51" t="s">
+        <v>269</v>
+      </c>
+      <c r="E518" s="50" t="s">
+        <v>266</v>
+      </c>
+      <c r="F518" s="73" t="s">
+        <v>270</v>
+      </c>
+      <c r="G518" s="46" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="519" spans="4:7">
+      <c r="D519" s="46"/>
+      <c r="E519" s="76"/>
+      <c r="F519" s="74"/>
+      <c r="G519" s="46"/>
+    </row>
+    <row r="520" spans="4:7">
+      <c r="D520" s="47"/>
+      <c r="E520" s="76"/>
+      <c r="F520" s="75"/>
+      <c r="G520" s="47"/>
+    </row>
+    <row r="521" spans="4:7">
+      <c r="D521" s="51" t="s">
+        <v>272</v>
+      </c>
+      <c r="E521" s="45" t="s">
+        <v>292</v>
+      </c>
+      <c r="F521" s="51"/>
+      <c r="G521" s="58" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="522" spans="4:7">
+      <c r="D522" s="46"/>
+      <c r="E522" s="46"/>
+      <c r="F522" s="46"/>
+      <c r="G522" s="71"/>
+    </row>
+    <row r="523" spans="4:7">
+      <c r="D523" s="46"/>
+      <c r="E523" s="46"/>
+      <c r="F523" s="46"/>
+      <c r="G523" s="71"/>
+    </row>
+    <row r="524" spans="4:7">
+      <c r="D524" s="46"/>
+      <c r="E524" s="46"/>
+      <c r="F524" s="46"/>
+      <c r="G524" s="71"/>
+    </row>
+    <row r="525" spans="4:7">
+      <c r="D525" s="47"/>
+      <c r="E525" s="47"/>
+      <c r="F525" s="47"/>
+      <c r="G525" s="72"/>
+    </row>
+    <row r="526" spans="4:7">
+      <c r="D526" s="51" t="s">
+        <v>275</v>
+      </c>
+      <c r="E526" s="58" t="s">
+        <v>276</v>
+      </c>
+      <c r="F526" s="64"/>
+      <c r="G526" s="58" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="527" spans="4:7">
+      <c r="D527" s="46"/>
+      <c r="E527" s="59"/>
+      <c r="F527" s="65"/>
+      <c r="G527" s="71"/>
+    </row>
+    <row r="528" spans="4:7">
+      <c r="D528" s="46"/>
+      <c r="E528" s="59"/>
+      <c r="F528" s="65"/>
+      <c r="G528" s="71"/>
+    </row>
+    <row r="529" spans="1:7">
+      <c r="D529" s="46"/>
+      <c r="E529" s="59"/>
+      <c r="F529" s="65"/>
+      <c r="G529" s="71"/>
+    </row>
+    <row r="530" spans="1:7">
+      <c r="D530" s="47"/>
+      <c r="E530" s="60"/>
+      <c r="F530" s="66"/>
+      <c r="G530" s="72"/>
+    </row>
+    <row r="531" spans="1:7">
+      <c r="D531" s="46" t="s">
+        <v>278</v>
+      </c>
+      <c r="E531" s="55" t="s">
+        <v>276</v>
+      </c>
+      <c r="F531" s="61"/>
+      <c r="G531" s="58" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="532" spans="1:7">
+      <c r="D532" s="46"/>
+      <c r="E532" s="56"/>
+      <c r="F532" s="62"/>
+      <c r="G532" s="59"/>
+    </row>
+    <row r="533" spans="1:7">
+      <c r="D533" s="46"/>
+      <c r="E533" s="56"/>
+      <c r="F533" s="62"/>
+      <c r="G533" s="59"/>
+    </row>
+    <row r="534" spans="1:7">
+      <c r="D534" s="47"/>
+      <c r="E534" s="57"/>
+      <c r="F534" s="63"/>
+      <c r="G534" s="60"/>
+    </row>
+    <row r="535" spans="1:7">
+      <c r="D535" s="51" t="s">
+        <v>280</v>
+      </c>
+      <c r="E535" s="58" t="s">
+        <v>281</v>
+      </c>
+      <c r="F535" s="58" t="s">
+        <v>282</v>
+      </c>
+      <c r="G535" s="58" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="536" spans="1:7" ht="26.25">
+      <c r="C536" s="20"/>
+      <c r="D536" s="46"/>
+      <c r="E536" s="59"/>
+      <c r="F536" s="71"/>
+      <c r="G536" s="71"/>
+    </row>
+    <row r="537" spans="1:7">
+      <c r="D537" s="46"/>
+      <c r="E537" s="59"/>
+      <c r="F537" s="71"/>
+      <c r="G537" s="71"/>
+    </row>
+    <row r="538" spans="1:7" ht="26.25">
       <c r="B538" s="20" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="539" spans="1:2">
+      <c r="D538" s="47"/>
+      <c r="E538" s="60"/>
+      <c r="F538" s="72"/>
+      <c r="G538" s="72"/>
+    </row>
+    <row r="539" spans="1:7">
       <c r="A539" t="s">
-        <v>280</v>
+        <v>293</v>
       </c>
       <c r="B539" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="540" spans="1:2">
+        <v>294</v>
+      </c>
+      <c r="D539" s="51" t="s">
+        <v>284</v>
+      </c>
+      <c r="E539" s="52" t="s">
+        <v>285</v>
+      </c>
+      <c r="F539" s="61"/>
+      <c r="G539" s="58" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="540" spans="1:7">
       <c r="B540" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="541" spans="1:2">
+        <v>295</v>
+      </c>
+      <c r="D540" s="46"/>
+      <c r="E540" s="53"/>
+      <c r="F540" s="62"/>
+      <c r="G540" s="71"/>
+    </row>
+    <row r="541" spans="1:7">
       <c r="B541" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="542" spans="1:2">
+        <v>296</v>
+      </c>
+      <c r="D541" s="46"/>
+      <c r="E541" s="53"/>
+      <c r="F541" s="62"/>
+      <c r="G541" s="71"/>
+    </row>
+    <row r="542" spans="1:7">
       <c r="B542" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="546" spans="2:2">
+        <v>297</v>
+      </c>
+      <c r="D542" s="47"/>
+      <c r="E542" s="54"/>
+      <c r="F542" s="63"/>
+      <c r="G542" s="72"/>
+    </row>
+    <row r="543" spans="1:7">
+      <c r="D543" s="51" t="s">
+        <v>287</v>
+      </c>
+      <c r="E543" s="55" t="s">
+        <v>288</v>
+      </c>
+      <c r="F543" s="67" t="s">
+        <v>289</v>
+      </c>
+      <c r="G543" s="58" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="544" spans="1:7">
+      <c r="D544" s="46"/>
+      <c r="E544" s="56"/>
+      <c r="F544" s="59"/>
+      <c r="G544" s="59"/>
+    </row>
+    <row r="545" spans="2:7">
+      <c r="D545" s="46"/>
+      <c r="E545" s="56"/>
+      <c r="F545" s="59"/>
+      <c r="G545" s="59"/>
+    </row>
+    <row r="546" spans="2:7" ht="26.25">
       <c r="B546" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="548" spans="2:2" ht="26.25">
+        <v>298</v>
+      </c>
+      <c r="C546" s="20"/>
+      <c r="D546" s="47"/>
+      <c r="E546" s="57"/>
+      <c r="F546" s="60"/>
+      <c r="G546" s="60"/>
+    </row>
+    <row r="548" spans="2:7" ht="26.25">
       <c r="B548" s="20"/>
     </row>
-    <row r="554" spans="2:2">
+    <row r="554" spans="2:7">
       <c r="B554" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="556" spans="2:2">
+    <row r="556" spans="2:7">
       <c r="B556" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="557" spans="2:2">
+    <row r="557" spans="2:7">
       <c r="B557" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="558" spans="2:2">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="558" spans="2:7">
       <c r="B558" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="559" spans="2:2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="559" spans="2:7">
       <c r="B559" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="560" spans="2:2">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="560" spans="2:7">
       <c r="B560" t="s">
-        <v>289</v>
+        <v>302</v>
       </c>
     </row>
     <row r="561" spans="2:2">
@@ -31455,7 +32294,7 @@
     </row>
     <row r="562" spans="2:2">
       <c r="B562" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
     </row>
     <row r="563" spans="2:2">
@@ -31465,22 +32304,22 @@
     </row>
     <row r="564" spans="2:2">
       <c r="B564" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
     </row>
     <row r="565" spans="2:2">
       <c r="B565" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
     </row>
     <row r="566" spans="2:2">
       <c r="B566" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
     </row>
     <row r="567" spans="2:2">
       <c r="B567" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
     </row>
     <row r="569" spans="2:2">
@@ -31490,7 +32329,7 @@
     </row>
     <row r="570" spans="2:2">
       <c r="B570" t="s">
-        <v>269</v>
+        <v>280</v>
       </c>
     </row>
     <row r="571" spans="2:2">
@@ -31500,17 +32339,17 @@
     </row>
     <row r="572" spans="2:2">
       <c r="B572" t="s">
-        <v>290</v>
+        <v>303</v>
       </c>
     </row>
     <row r="573" spans="2:2">
       <c r="B573" t="s">
-        <v>291</v>
+        <v>304</v>
       </c>
     </row>
     <row r="574" spans="2:2">
       <c r="B574" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
     </row>
     <row r="575" spans="2:2">
@@ -31520,12 +32359,12 @@
     </row>
     <row r="577" spans="2:2">
       <c r="B577" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
     </row>
     <row r="578" spans="2:2">
       <c r="B578" t="s">
-        <v>293</v>
+        <v>306</v>
       </c>
     </row>
     <row r="581" spans="2:2">
@@ -31535,11 +32374,47 @@
     </row>
     <row r="585" spans="2:2">
       <c r="B585" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="72">
+    <mergeCell ref="D543:D546"/>
+    <mergeCell ref="E543:E546"/>
+    <mergeCell ref="F543:F546"/>
+    <mergeCell ref="G543:G546"/>
+    <mergeCell ref="D535:D538"/>
+    <mergeCell ref="E535:E538"/>
+    <mergeCell ref="F535:F538"/>
+    <mergeCell ref="G535:G538"/>
+    <mergeCell ref="D539:D542"/>
+    <mergeCell ref="E539:E542"/>
+    <mergeCell ref="F539:F542"/>
+    <mergeCell ref="G539:G542"/>
+    <mergeCell ref="D526:D530"/>
+    <mergeCell ref="E526:E530"/>
+    <mergeCell ref="F526:F530"/>
+    <mergeCell ref="G526:G530"/>
+    <mergeCell ref="D531:D534"/>
+    <mergeCell ref="E531:E534"/>
+    <mergeCell ref="F531:F534"/>
+    <mergeCell ref="G531:G534"/>
+    <mergeCell ref="D518:D520"/>
+    <mergeCell ref="E518:E520"/>
+    <mergeCell ref="F518:F520"/>
+    <mergeCell ref="G518:G520"/>
+    <mergeCell ref="D521:D525"/>
+    <mergeCell ref="E521:E525"/>
+    <mergeCell ref="F521:F525"/>
+    <mergeCell ref="G521:G525"/>
+    <mergeCell ref="D509:D512"/>
+    <mergeCell ref="E509:E512"/>
+    <mergeCell ref="F509:F512"/>
+    <mergeCell ref="G509:G512"/>
+    <mergeCell ref="D513:D517"/>
+    <mergeCell ref="E513:E517"/>
+    <mergeCell ref="F513:F517"/>
+    <mergeCell ref="G513:G517"/>
     <mergeCell ref="F488:F491"/>
     <mergeCell ref="F475:F479"/>
     <mergeCell ref="E480:E483"/>
@@ -31586,7 +32461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B55294-0735-4753-AFC3-1794F1BD4C0C}">
   <dimension ref="A1:O187"/>
   <sheetViews>
-    <sheetView topLeftCell="A170" workbookViewId="0">
+    <sheetView topLeftCell="A200" workbookViewId="0">
       <selection activeCell="B179" sqref="B179:C179"/>
     </sheetView>
   </sheetViews>
@@ -31603,16 +32478,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="3" t="s">
-        <v>295</v>
+        <v>308</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>296</v>
+        <v>309</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>297</v>
+        <v>310</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>298</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -31620,13 +32495,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="C2" t="s">
-        <v>300</v>
+        <v>313</v>
       </c>
       <c r="D2" t="s">
-        <v>301</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -31634,13 +32509,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="C3" t="s">
-        <v>302</v>
+        <v>315</v>
       </c>
       <c r="D3" t="s">
-        <v>303</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -31648,13 +32523,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="C4" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="D4" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -31662,13 +32537,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="C5" t="s">
-        <v>306</v>
+        <v>319</v>
       </c>
       <c r="D5" t="s">
-        <v>307</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -31676,18 +32551,18 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="C6" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="D6" t="s">
-        <v>308</v>
+        <v>321</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="21">
       <c r="B18" s="4" t="s">
-        <v>309</v>
+        <v>322</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -31722,99 +32597,99 @@
     </row>
     <row r="32" spans="1:12">
       <c r="B32" s="5" t="s">
-        <v>295</v>
+        <v>308</v>
       </c>
       <c r="C32" t="s">
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>297</v>
+        <v>310</v>
       </c>
       <c r="E32" t="s">
-        <v>298</v>
+        <v>311</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>310</v>
+        <v>323</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="B33" s="5" t="s">
-        <v>311</v>
+        <v>324</v>
       </c>
       <c r="C33" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="D33" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="E33" t="s">
-        <v>313</v>
+        <v>326</v>
       </c>
       <c r="G33" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="14" customFormat="1">
       <c r="C34" s="14" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>316</v>
+        <v>329</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>317</v>
+        <v>330</v>
       </c>
     </row>
     <row r="35" spans="1:7" s="15" customFormat="1">
       <c r="A35" s="15" t="s">
-        <v>318</v>
+        <v>331</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>320</v>
+        <v>333</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="C36" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="D36" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="E36" t="s">
-        <v>323</v>
+        <v>336</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="D37" t="s">
-        <v>324</v>
+        <v>337</v>
       </c>
       <c r="E37" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="E42" s="12" t="s">
-        <v>309</v>
+        <v>322</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="12" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -31822,7 +32697,7 @@
         <v>1</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -31830,7 +32705,7 @@
         <v>2</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>328</v>
+        <v>341</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -31838,7 +32713,7 @@
         <v>3</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
     </row>
     <row r="68" spans="1:14" ht="28.5" customHeight="1">
@@ -31877,16 +32752,16 @@
     </row>
     <row r="77" spans="1:14">
       <c r="B77" s="5" t="s">
-        <v>295</v>
+        <v>308</v>
       </c>
       <c r="C77" t="s">
         <v>1</v>
       </c>
       <c r="D77" t="s">
-        <v>297</v>
+        <v>310</v>
       </c>
       <c r="E77" t="s">
-        <v>298</v>
+        <v>311</v>
       </c>
     </row>
     <row r="78" spans="1:14">
@@ -31895,13 +32770,13 @@
         <v>1</v>
       </c>
       <c r="C78" s="24" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="D78" s="24" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="E78" s="24" t="s">
-        <v>313</v>
+        <v>326</v>
       </c>
     </row>
     <row r="79" spans="1:14">
@@ -31910,13 +32785,13 @@
         <v>2</v>
       </c>
       <c r="C79" s="24" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="D79" s="24" t="s">
-        <v>330</v>
+        <v>343</v>
       </c>
       <c r="E79" s="24" t="s">
-        <v>331</v>
+        <v>344</v>
       </c>
     </row>
     <row r="80" spans="1:14">
@@ -31925,13 +32800,13 @@
         <v>3</v>
       </c>
       <c r="C80" s="24" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="D80" s="24" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
       <c r="E80" s="24" t="s">
-        <v>320</v>
+        <v>333</v>
       </c>
     </row>
     <row r="81" spans="2:5">
@@ -31939,13 +32814,13 @@
         <v>4</v>
       </c>
       <c r="C81" s="24" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="D81" s="24" t="s">
-        <v>332</v>
+        <v>345</v>
       </c>
       <c r="E81" s="24" t="s">
-        <v>323</v>
+        <v>336</v>
       </c>
     </row>
     <row r="87" spans="2:5">
@@ -31989,10 +32864,10 @@
     </row>
     <row r="176" spans="1:15">
       <c r="B176" s="34" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="C176" s="35" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="D176" s="36" t="s">
         <v>35</v>
@@ -32003,35 +32878,35 @@
     </row>
     <row r="177" spans="2:5">
       <c r="B177" s="33" t="s">
-        <v>333</v>
+        <v>346</v>
       </c>
       <c r="C177" s="28" t="s">
-        <v>334</v>
+        <v>347</v>
       </c>
       <c r="D177" s="32" t="s">
-        <v>335</v>
+        <v>348</v>
       </c>
       <c r="E177" s="31" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
     </row>
     <row r="178" spans="2:5">
       <c r="B178" s="33"/>
       <c r="C178" s="28" t="s">
-        <v>337</v>
+        <v>350</v>
       </c>
       <c r="D178" s="32" t="s">
-        <v>338</v>
+        <v>351</v>
       </c>
       <c r="E178" s="31"/>
     </row>
     <row r="179" spans="2:5">
       <c r="B179" s="38"/>
       <c r="C179" s="28" t="s">
-        <v>339</v>
+        <v>352</v>
       </c>
       <c r="D179" s="40" t="s">
-        <v>340</v>
+        <v>353</v>
       </c>
       <c r="E179" s="41"/>
     </row>
@@ -32043,25 +32918,25 @@
     </row>
     <row r="181" spans="2:5">
       <c r="B181" s="33" t="s">
-        <v>341</v>
+        <v>354</v>
       </c>
       <c r="C181" s="28" t="s">
-        <v>342</v>
+        <v>355</v>
       </c>
       <c r="D181" s="32" t="s">
-        <v>343</v>
+        <v>356</v>
       </c>
       <c r="E181" s="31" t="s">
-        <v>344</v>
+        <v>357</v>
       </c>
     </row>
     <row r="182" spans="2:5">
       <c r="B182" s="33"/>
       <c r="C182" s="30" t="s">
-        <v>345</v>
+        <v>358</v>
       </c>
       <c r="D182" s="32" t="s">
-        <v>346</v>
+        <v>359</v>
       </c>
       <c r="E182" s="31"/>
     </row>
@@ -32073,23 +32948,23 @@
     </row>
     <row r="184" spans="2:5">
       <c r="B184" s="33" t="s">
-        <v>347</v>
+        <v>360</v>
       </c>
       <c r="C184" s="28" t="s">
-        <v>348</v>
+        <v>361</v>
       </c>
       <c r="D184" s="32" t="s">
-        <v>349</v>
+        <v>362</v>
       </c>
       <c r="E184" s="31"/>
     </row>
     <row r="185" spans="2:5">
       <c r="B185" s="33"/>
       <c r="C185" s="28" t="s">
-        <v>350</v>
+        <v>363</v>
       </c>
       <c r="D185" s="32" t="s">
-        <v>351</v>
+        <v>364</v>
       </c>
       <c r="E185" s="31"/>
     </row>
@@ -32101,12 +32976,12 @@
     </row>
     <row r="187" spans="2:5">
       <c r="B187" s="38" t="s">
-        <v>352</v>
+        <v>365</v>
       </c>
       <c r="C187" s="39"/>
       <c r="D187" s="40"/>
       <c r="E187" s="41" t="s">
-        <v>353</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -32140,7 +33015,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>354</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75">
@@ -32162,13 +33037,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>355</v>
+        <v>368</v>
       </c>
       <c r="C4" t="s">
-        <v>356</v>
+        <v>369</v>
       </c>
       <c r="D4" t="s">
-        <v>357</v>
+        <v>370</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -32176,13 +33051,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>355</v>
+        <v>368</v>
       </c>
       <c r="C5" t="s">
-        <v>358</v>
+        <v>371</v>
       </c>
       <c r="D5" t="s">
-        <v>359</v>
+        <v>372</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -32190,13 +33065,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>355</v>
+        <v>368</v>
       </c>
       <c r="C6" t="s">
-        <v>360</v>
+        <v>373</v>
       </c>
       <c r="D6" t="s">
-        <v>361</v>
+        <v>374</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -32204,13 +33079,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>362</v>
+        <v>375</v>
       </c>
       <c r="C7" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="D7" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -32218,13 +33093,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>362</v>
+        <v>375</v>
       </c>
       <c r="C8" t="s">
-        <v>365</v>
+        <v>378</v>
       </c>
       <c r="D8" t="s">
-        <v>366</v>
+        <v>379</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -32232,13 +33107,13 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>362</v>
+        <v>375</v>
       </c>
       <c r="C9" t="s">
-        <v>367</v>
+        <v>380</v>
       </c>
       <c r="D9" t="s">
-        <v>368</v>
+        <v>381</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -32246,13 +33121,13 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>362</v>
+        <v>375</v>
       </c>
       <c r="C10" t="s">
-        <v>369</v>
+        <v>382</v>
       </c>
       <c r="D10" t="s">
-        <v>370</v>
+        <v>383</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -32260,13 +33135,13 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>362</v>
+        <v>375</v>
       </c>
       <c r="C11" t="s">
-        <v>371</v>
+        <v>384</v>
       </c>
       <c r="D11" t="s">
-        <v>372</v>
+        <v>385</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -32274,13 +33149,13 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>362</v>
+        <v>375</v>
       </c>
       <c r="C12" t="s">
-        <v>373</v>
+        <v>386</v>
       </c>
       <c r="D12" t="s">
-        <v>374</v>
+        <v>387</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -32288,13 +33163,13 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>362</v>
+        <v>375</v>
       </c>
       <c r="C13" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="D13" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -32302,13 +33177,13 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>375</v>
+        <v>388</v>
       </c>
       <c r="C14" t="s">
-        <v>376</v>
+        <v>389</v>
       </c>
       <c r="D14" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -32316,13 +33191,13 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>375</v>
+        <v>388</v>
       </c>
       <c r="C15" t="s">
-        <v>378</v>
+        <v>391</v>
       </c>
       <c r="D15" t="s">
-        <v>379</v>
+        <v>392</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18.75">
@@ -32332,7 +33207,7 @@
     </row>
     <row r="22" spans="1:5" ht="18.75">
       <c r="B22" s="1" t="s">
-        <v>355</v>
+        <v>368</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="18.75">
@@ -32340,7 +33215,7 @@
     </row>
     <row r="34" spans="1:17" ht="21">
       <c r="B34" s="4" t="s">
-        <v>362</v>
+        <v>375</v>
       </c>
     </row>
     <row r="41" spans="1:17" ht="29.25" customHeight="1">
@@ -32419,35 +33294,35 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>381</v>
+        <v>394</v>
       </c>
       <c r="B2" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>383</v>
+        <v>396</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>384</v>
+        <v>397</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>385</v>
+        <v>398</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="39" customHeight="1">
       <c r="A9" s="17" t="s">
-        <v>386</v>
+        <v>399</v>
       </c>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -32467,7 +33342,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32477,10 +33352,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>388</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -32489,4 +33364,19 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5126D9-BF4E-45A4-8244-D1997D77AADD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>